<commit_message>
Added bulk build hearing days for NVHQ
</commit_message>
<xml_diff>
--- a/public/ROAssignmentTemplate.xlsx
+++ b/public/ROAssignmentTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navaloaner_2/workspace/caseflow/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695AB6D3-09A9-E041-84F7-583CFC741760}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1CBF7A-C1BD-B345-A313-3D37E92C1DDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16700" yWindow="2460" windowWidth="19580" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="124">
   <si>
     <t>Example</t>
   </si>
@@ -388,6 +388,12 @@
   </si>
   <si>
     <t>Number of Hearing Days with 425 I Rooms Allocated in Date Range</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>NVHQ</t>
   </si>
 </sst>
 </file>
@@ -397,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -407,16 +413,19 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -428,38 +437,55 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Source Sans Pro"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -512,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -615,21 +641,6 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -961,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,32 +1007,32 @@
     <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1032,9 +1043,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1049,29 +1060,41 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1084,28 +1107,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2298,7 +2311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IT50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BF4" sqref="BF4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2308,27 +2323,29 @@
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="254" width="11" style="1" customWidth="1"/>
+    <col min="7" max="57" width="11" style="1" customWidth="1"/>
+    <col min="58" max="58" width="11" style="43" customWidth="1"/>
+    <col min="59" max="254" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2373,8 +2390,9 @@
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
       <c r="BE1" s="5"/>
-    </row>
-    <row r="2" spans="1:57" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF1" s="5"/>
+    </row>
+    <row r="2" spans="1:58" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2546,8 +2564,11 @@
       <c r="BE2" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:57" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF2" s="86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2719,433 +2740,443 @@
       <c r="BE3" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:57" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF3" s="85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="15">
         <v>43466</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="75"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="75"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="75"/>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="75"/>
-      <c r="AC4" s="75"/>
-      <c r="AD4" s="75"/>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="75"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="75"/>
-      <c r="AK4" s="75"/>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="75"/>
-      <c r="AN4" s="75"/>
-      <c r="AO4" s="75"/>
-      <c r="AP4" s="75"/>
-      <c r="AQ4" s="75"/>
-      <c r="AR4" s="75"/>
-      <c r="AS4" s="75"/>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="75"/>
-      <c r="AY4" s="75"/>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="75"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="75"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="75"/>
-    </row>
-    <row r="5" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="67"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="67"/>
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="67"/>
+      <c r="AE4" s="67"/>
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67"/>
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67"/>
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67"/>
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67"/>
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="67"/>
+      <c r="AU4" s="67"/>
+      <c r="AV4" s="67"/>
+      <c r="AW4" s="67"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="67"/>
+      <c r="AZ4" s="67"/>
+      <c r="BA4" s="67"/>
+      <c r="BB4" s="67"/>
+      <c r="BC4" s="67"/>
+      <c r="BD4" s="67"/>
+      <c r="BE4" s="67"/>
+      <c r="BF4" s="67"/>
+    </row>
+    <row r="5" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="18">
         <v>43497</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="78"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="78"/>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78"/>
-      <c r="AK5" s="78"/>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="78"/>
-      <c r="AN5" s="78"/>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="78"/>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="78"/>
-      <c r="AW5" s="78"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="78"/>
-      <c r="AZ5" s="78"/>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="78"/>
-      <c r="BC5" s="78"/>
-      <c r="BD5" s="78"/>
-      <c r="BE5" s="79"/>
-    </row>
-    <row r="6" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
+      <c r="AD5" s="70"/>
+      <c r="AE5" s="70"/>
+      <c r="AF5" s="70"/>
+      <c r="AG5" s="70"/>
+      <c r="AH5" s="70"/>
+      <c r="AI5" s="70"/>
+      <c r="AJ5" s="70"/>
+      <c r="AK5" s="70"/>
+      <c r="AL5" s="70"/>
+      <c r="AM5" s="70"/>
+      <c r="AN5" s="70"/>
+      <c r="AO5" s="70"/>
+      <c r="AP5" s="70"/>
+      <c r="AQ5" s="70"/>
+      <c r="AR5" s="70"/>
+      <c r="AS5" s="70"/>
+      <c r="AT5" s="70"/>
+      <c r="AU5" s="70"/>
+      <c r="AV5" s="70"/>
+      <c r="AW5" s="70"/>
+      <c r="AX5" s="70"/>
+      <c r="AY5" s="70"/>
+      <c r="AZ5" s="70"/>
+      <c r="BA5" s="70"/>
+      <c r="BB5" s="70"/>
+      <c r="BC5" s="70"/>
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="71"/>
+      <c r="BF5" s="71"/>
+    </row>
+    <row r="6" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="20">
         <v>43540</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
-      <c r="X6" s="82"/>
-      <c r="Y6" s="82"/>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="82"/>
-      <c r="AC6" s="82"/>
-      <c r="AD6" s="82"/>
-      <c r="AE6" s="82"/>
-      <c r="AF6" s="82"/>
-      <c r="AG6" s="82"/>
-      <c r="AH6" s="82"/>
-      <c r="AI6" s="82"/>
-      <c r="AJ6" s="82"/>
-      <c r="AK6" s="82"/>
-      <c r="AL6" s="82"/>
-      <c r="AM6" s="82"/>
-      <c r="AN6" s="82"/>
-      <c r="AO6" s="82"/>
-      <c r="AP6" s="82"/>
-      <c r="AQ6" s="82"/>
-      <c r="AR6" s="82"/>
-      <c r="AS6" s="82"/>
-      <c r="AT6" s="82"/>
-      <c r="AU6" s="82"/>
-      <c r="AV6" s="82"/>
-      <c r="AW6" s="82"/>
-      <c r="AX6" s="82"/>
-      <c r="AY6" s="82"/>
-      <c r="AZ6" s="82"/>
-      <c r="BA6" s="82"/>
-      <c r="BB6" s="82"/>
-      <c r="BC6" s="82"/>
-      <c r="BD6" s="82"/>
-      <c r="BE6" s="82"/>
-    </row>
-    <row r="7" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="72"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="74"/>
+      <c r="X6" s="74"/>
+      <c r="Y6" s="74"/>
+      <c r="Z6" s="74"/>
+      <c r="AA6" s="74"/>
+      <c r="AB6" s="74"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="74"/>
+      <c r="AE6" s="74"/>
+      <c r="AF6" s="74"/>
+      <c r="AG6" s="74"/>
+      <c r="AH6" s="74"/>
+      <c r="AI6" s="74"/>
+      <c r="AJ6" s="74"/>
+      <c r="AK6" s="74"/>
+      <c r="AL6" s="74"/>
+      <c r="AM6" s="74"/>
+      <c r="AN6" s="74"/>
+      <c r="AO6" s="74"/>
+      <c r="AP6" s="74"/>
+      <c r="AQ6" s="74"/>
+      <c r="AR6" s="74"/>
+      <c r="AS6" s="74"/>
+      <c r="AT6" s="74"/>
+      <c r="AU6" s="74"/>
+      <c r="AV6" s="74"/>
+      <c r="AW6" s="74"/>
+      <c r="AX6" s="74"/>
+      <c r="AY6" s="74"/>
+      <c r="AZ6" s="74"/>
+      <c r="BA6" s="74"/>
+      <c r="BB6" s="74"/>
+      <c r="BC6" s="74"/>
+      <c r="BD6" s="74"/>
+      <c r="BE6" s="74"/>
+      <c r="BF6" s="74"/>
+    </row>
+    <row r="7" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="21">
         <v>43576</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="78"/>
-      <c r="R7" s="78"/>
-      <c r="S7" s="78"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="78"/>
-      <c r="W7" s="78"/>
-      <c r="X7" s="78"/>
-      <c r="Y7" s="78"/>
-      <c r="Z7" s="78"/>
-      <c r="AA7" s="78"/>
-      <c r="AB7" s="78"/>
-      <c r="AC7" s="78"/>
-      <c r="AD7" s="78"/>
-      <c r="AE7" s="78"/>
-      <c r="AF7" s="78"/>
-      <c r="AG7" s="78"/>
-      <c r="AH7" s="78"/>
-      <c r="AI7" s="78"/>
-      <c r="AJ7" s="78"/>
-      <c r="AK7" s="78"/>
-      <c r="AL7" s="78"/>
-      <c r="AM7" s="78"/>
-      <c r="AN7" s="78"/>
-      <c r="AO7" s="78"/>
-      <c r="AP7" s="78"/>
-      <c r="AQ7" s="78"/>
-      <c r="AR7" s="78"/>
-      <c r="AS7" s="78"/>
-      <c r="AT7" s="78"/>
-      <c r="AU7" s="78"/>
-      <c r="AV7" s="78"/>
-      <c r="AW7" s="78"/>
-      <c r="AX7" s="78"/>
-      <c r="AY7" s="78"/>
-      <c r="AZ7" s="78"/>
-      <c r="BA7" s="78"/>
-      <c r="BB7" s="78"/>
-      <c r="BC7" s="78"/>
-      <c r="BD7" s="78"/>
-      <c r="BE7" s="79"/>
-    </row>
-    <row r="8" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="75"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+      <c r="S7" s="70"/>
+      <c r="T7" s="70"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="70"/>
+      <c r="X7" s="70"/>
+      <c r="Y7" s="70"/>
+      <c r="Z7" s="70"/>
+      <c r="AA7" s="70"/>
+      <c r="AB7" s="70"/>
+      <c r="AC7" s="70"/>
+      <c r="AD7" s="70"/>
+      <c r="AE7" s="70"/>
+      <c r="AF7" s="70"/>
+      <c r="AG7" s="70"/>
+      <c r="AH7" s="70"/>
+      <c r="AI7" s="70"/>
+      <c r="AJ7" s="70"/>
+      <c r="AK7" s="70"/>
+      <c r="AL7" s="70"/>
+      <c r="AM7" s="70"/>
+      <c r="AN7" s="70"/>
+      <c r="AO7" s="70"/>
+      <c r="AP7" s="70"/>
+      <c r="AQ7" s="70"/>
+      <c r="AR7" s="70"/>
+      <c r="AS7" s="70"/>
+      <c r="AT7" s="70"/>
+      <c r="AU7" s="70"/>
+      <c r="AV7" s="70"/>
+      <c r="AW7" s="70"/>
+      <c r="AX7" s="70"/>
+      <c r="AY7" s="70"/>
+      <c r="AZ7" s="70"/>
+      <c r="BA7" s="70"/>
+      <c r="BB7" s="70"/>
+      <c r="BC7" s="70"/>
+      <c r="BD7" s="70"/>
+      <c r="BE7" s="71"/>
+      <c r="BF7" s="71"/>
+    </row>
+    <row r="8" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="23">
         <v>43604</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="82"/>
-      <c r="R8" s="82"/>
-      <c r="S8" s="82"/>
-      <c r="T8" s="82"/>
-      <c r="U8" s="82"/>
-      <c r="V8" s="82"/>
-      <c r="W8" s="82"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="82"/>
-      <c r="Z8" s="82"/>
-      <c r="AA8" s="82"/>
-      <c r="AB8" s="82"/>
-      <c r="AC8" s="82"/>
-      <c r="AD8" s="82"/>
-      <c r="AE8" s="82"/>
-      <c r="AF8" s="82"/>
-      <c r="AG8" s="82"/>
-      <c r="AH8" s="82"/>
-      <c r="AI8" s="82"/>
-      <c r="AJ8" s="82"/>
-      <c r="AK8" s="82"/>
-      <c r="AL8" s="82"/>
-      <c r="AM8" s="82"/>
-      <c r="AN8" s="82"/>
-      <c r="AO8" s="82"/>
-      <c r="AP8" s="82"/>
-      <c r="AQ8" s="82"/>
-      <c r="AR8" s="82"/>
-      <c r="AS8" s="82"/>
-      <c r="AT8" s="82"/>
-      <c r="AU8" s="82"/>
-      <c r="AV8" s="82"/>
-      <c r="AW8" s="82"/>
-      <c r="AX8" s="82"/>
-      <c r="AY8" s="82"/>
-      <c r="AZ8" s="82"/>
-      <c r="BA8" s="82"/>
-      <c r="BB8" s="82"/>
-      <c r="BC8" s="82"/>
-      <c r="BD8" s="82"/>
-      <c r="BE8" s="82"/>
-    </row>
-    <row r="9" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="76"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74"/>
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="74"/>
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74"/>
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="74"/>
+      <c r="AW8" s="74"/>
+      <c r="AX8" s="74"/>
+      <c r="AY8" s="74"/>
+      <c r="AZ8" s="74"/>
+      <c r="BA8" s="74"/>
+      <c r="BB8" s="74"/>
+      <c r="BC8" s="74"/>
+      <c r="BD8" s="74"/>
+      <c r="BE8" s="74"/>
+      <c r="BF8" s="74"/>
+    </row>
+    <row r="9" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78"/>
-      <c r="X9" s="78"/>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78"/>
-      <c r="AB9" s="78"/>
-      <c r="AC9" s="78"/>
-      <c r="AD9" s="78"/>
-      <c r="AE9" s="78"/>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="78"/>
-      <c r="AH9" s="78"/>
-      <c r="AI9" s="78"/>
-      <c r="AJ9" s="78"/>
-      <c r="AK9" s="78"/>
-      <c r="AL9" s="78"/>
-      <c r="AM9" s="78"/>
-      <c r="AN9" s="78"/>
-      <c r="AO9" s="78"/>
-      <c r="AP9" s="78"/>
-      <c r="AQ9" s="78"/>
-      <c r="AR9" s="78"/>
-      <c r="AS9" s="78"/>
-      <c r="AT9" s="78"/>
-      <c r="AU9" s="78"/>
-      <c r="AV9" s="78"/>
-      <c r="AW9" s="78"/>
-      <c r="AX9" s="78"/>
-      <c r="AY9" s="78"/>
-      <c r="AZ9" s="78"/>
-      <c r="BA9" s="78"/>
-      <c r="BB9" s="78"/>
-      <c r="BC9" s="78"/>
-      <c r="BD9" s="78"/>
-      <c r="BE9" s="79"/>
-    </row>
-    <row r="10" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="77"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
+      <c r="Y9" s="70"/>
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="70"/>
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="70"/>
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="70"/>
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="70"/>
+      <c r="AH9" s="70"/>
+      <c r="AI9" s="70"/>
+      <c r="AJ9" s="70"/>
+      <c r="AK9" s="70"/>
+      <c r="AL9" s="70"/>
+      <c r="AM9" s="70"/>
+      <c r="AN9" s="70"/>
+      <c r="AO9" s="70"/>
+      <c r="AP9" s="70"/>
+      <c r="AQ9" s="70"/>
+      <c r="AR9" s="70"/>
+      <c r="AS9" s="70"/>
+      <c r="AT9" s="70"/>
+      <c r="AU9" s="70"/>
+      <c r="AV9" s="70"/>
+      <c r="AW9" s="70"/>
+      <c r="AX9" s="70"/>
+      <c r="AY9" s="70"/>
+      <c r="AZ9" s="70"/>
+      <c r="BA9" s="70"/>
+      <c r="BB9" s="70"/>
+      <c r="BC9" s="70"/>
+      <c r="BD9" s="70"/>
+      <c r="BE9" s="71"/>
+      <c r="BF9" s="71"/>
+    </row>
+    <row r="10" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="82"/>
-      <c r="T10" s="82"/>
-      <c r="U10" s="82"/>
-      <c r="V10" s="82"/>
-      <c r="W10" s="82"/>
-      <c r="X10" s="82"/>
-      <c r="Y10" s="82"/>
-      <c r="Z10" s="82"/>
-      <c r="AA10" s="82"/>
-      <c r="AB10" s="82"/>
-      <c r="AC10" s="82"/>
-      <c r="AD10" s="82"/>
-      <c r="AE10" s="82"/>
-      <c r="AF10" s="82"/>
-      <c r="AG10" s="82"/>
-      <c r="AH10" s="82"/>
-      <c r="AI10" s="82"/>
-      <c r="AJ10" s="82"/>
-      <c r="AK10" s="82"/>
-      <c r="AL10" s="82"/>
-      <c r="AM10" s="82"/>
-      <c r="AN10" s="82"/>
-      <c r="AO10" s="82"/>
-      <c r="AP10" s="82"/>
-      <c r="AQ10" s="82"/>
-      <c r="AR10" s="82"/>
-      <c r="AS10" s="82"/>
-      <c r="AT10" s="82"/>
-      <c r="AU10" s="82"/>
-      <c r="AV10" s="82"/>
-      <c r="AW10" s="82"/>
-      <c r="AX10" s="82"/>
-      <c r="AY10" s="82"/>
-      <c r="AZ10" s="82"/>
-      <c r="BA10" s="82"/>
-      <c r="BB10" s="82"/>
-      <c r="BC10" s="82"/>
-      <c r="BD10" s="82"/>
-      <c r="BE10" s="82"/>
-    </row>
-    <row r="11" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="76"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="74"/>
+      <c r="AC10" s="74"/>
+      <c r="AD10" s="74"/>
+      <c r="AE10" s="74"/>
+      <c r="AF10" s="74"/>
+      <c r="AG10" s="74"/>
+      <c r="AH10" s="74"/>
+      <c r="AI10" s="74"/>
+      <c r="AJ10" s="74"/>
+      <c r="AK10" s="74"/>
+      <c r="AL10" s="74"/>
+      <c r="AM10" s="74"/>
+      <c r="AN10" s="74"/>
+      <c r="AO10" s="74"/>
+      <c r="AP10" s="74"/>
+      <c r="AQ10" s="74"/>
+      <c r="AR10" s="74"/>
+      <c r="AS10" s="74"/>
+      <c r="AT10" s="74"/>
+      <c r="AU10" s="74"/>
+      <c r="AV10" s="74"/>
+      <c r="AW10" s="74"/>
+      <c r="AX10" s="74"/>
+      <c r="AY10" s="74"/>
+      <c r="AZ10" s="74"/>
+      <c r="BA10" s="74"/>
+      <c r="BB10" s="74"/>
+      <c r="BC10" s="74"/>
+      <c r="BD10" s="74"/>
+      <c r="BE10" s="74"/>
+      <c r="BF10" s="74"/>
+    </row>
+    <row r="11" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" s="27"/>
       <c r="C11" s="24"/>
@@ -3203,8 +3234,9 @@
       <c r="BC11" s="24"/>
       <c r="BD11" s="24"/>
       <c r="BE11" s="28"/>
-    </row>
-    <row r="12" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF11" s="28"/>
+    </row>
+    <row r="12" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
@@ -3262,8 +3294,9 @@
       <c r="BC12" s="26"/>
       <c r="BD12" s="26"/>
       <c r="BE12" s="26"/>
-    </row>
-    <row r="13" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF12" s="26"/>
+    </row>
+    <row r="13" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
       <c r="C13" s="29"/>
@@ -3321,8 +3354,9 @@
       <c r="BC13" s="29"/>
       <c r="BD13" s="29"/>
       <c r="BE13" s="30"/>
-    </row>
-    <row r="14" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF13" s="30"/>
+    </row>
+    <row r="14" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="25"/>
       <c r="C14" s="31"/>
@@ -3380,8 +3414,9 @@
       <c r="BC14" s="31"/>
       <c r="BD14" s="31"/>
       <c r="BE14" s="31"/>
-    </row>
-    <row r="15" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF14" s="31"/>
+    </row>
+    <row r="15" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
       <c r="C15" s="29"/>
@@ -3439,8 +3474,9 @@
       <c r="BC15" s="29"/>
       <c r="BD15" s="29"/>
       <c r="BE15" s="30"/>
-    </row>
-    <row r="16" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF15" s="30"/>
+    </row>
+    <row r="16" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="25"/>
       <c r="C16" s="31"/>
@@ -3498,8 +3534,9 @@
       <c r="BC16" s="31"/>
       <c r="BD16" s="31"/>
       <c r="BE16" s="31"/>
-    </row>
-    <row r="17" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF16" s="31"/>
+    </row>
+    <row r="17" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="27"/>
       <c r="C17" s="29"/>
@@ -3557,8 +3594,9 @@
       <c r="BC17" s="29"/>
       <c r="BD17" s="29"/>
       <c r="BE17" s="30"/>
-    </row>
-    <row r="18" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF17" s="30"/>
+    </row>
+    <row r="18" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="25"/>
       <c r="C18" s="31"/>
@@ -3616,8 +3654,9 @@
       <c r="BC18" s="31"/>
       <c r="BD18" s="31"/>
       <c r="BE18" s="31"/>
-    </row>
-    <row r="19" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF18" s="31"/>
+    </row>
+    <row r="19" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
       <c r="C19" s="29"/>
@@ -3675,8 +3714,9 @@
       <c r="BC19" s="29"/>
       <c r="BD19" s="29"/>
       <c r="BE19" s="30"/>
-    </row>
-    <row r="20" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF19" s="30"/>
+    </row>
+    <row r="20" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="25"/>
       <c r="C20" s="31"/>
@@ -3734,8 +3774,9 @@
       <c r="BC20" s="31"/>
       <c r="BD20" s="31"/>
       <c r="BE20" s="31"/>
-    </row>
-    <row r="21" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF20" s="31"/>
+    </row>
+    <row r="21" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="27"/>
       <c r="C21" s="29"/>
@@ -3793,8 +3834,9 @@
       <c r="BC21" s="29"/>
       <c r="BD21" s="29"/>
       <c r="BE21" s="30"/>
-    </row>
-    <row r="22" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF21" s="30"/>
+    </row>
+    <row r="22" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="25"/>
       <c r="C22" s="31"/>
@@ -3852,8 +3894,9 @@
       <c r="BC22" s="31"/>
       <c r="BD22" s="31"/>
       <c r="BE22" s="31"/>
-    </row>
-    <row r="23" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF22" s="31"/>
+    </row>
+    <row r="23" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="27"/>
       <c r="C23" s="29"/>
@@ -3911,8 +3954,9 @@
       <c r="BC23" s="29"/>
       <c r="BD23" s="29"/>
       <c r="BE23" s="30"/>
-    </row>
-    <row r="24" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF23" s="30"/>
+    </row>
+    <row r="24" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="25"/>
       <c r="C24" s="31"/>
@@ -3970,8 +4014,9 @@
       <c r="BC24" s="31"/>
       <c r="BD24" s="31"/>
       <c r="BE24" s="31"/>
-    </row>
-    <row r="25" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF24" s="31"/>
+    </row>
+    <row r="25" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="27"/>
       <c r="C25" s="29"/>
@@ -4029,8 +4074,9 @@
       <c r="BC25" s="29"/>
       <c r="BD25" s="29"/>
       <c r="BE25" s="30"/>
-    </row>
-    <row r="26" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF25" s="30"/>
+    </row>
+    <row r="26" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="25"/>
       <c r="C26" s="31"/>
@@ -4088,8 +4134,9 @@
       <c r="BC26" s="31"/>
       <c r="BD26" s="31"/>
       <c r="BE26" s="31"/>
-    </row>
-    <row r="27" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF26" s="31"/>
+    </row>
+    <row r="27" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="27"/>
       <c r="C27" s="29"/>
@@ -4147,8 +4194,9 @@
       <c r="BC27" s="29"/>
       <c r="BD27" s="29"/>
       <c r="BE27" s="30"/>
-    </row>
-    <row r="28" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF27" s="30"/>
+    </row>
+    <row r="28" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="25"/>
       <c r="C28" s="31"/>
@@ -4206,8 +4254,9 @@
       <c r="BC28" s="31"/>
       <c r="BD28" s="31"/>
       <c r="BE28" s="31"/>
-    </row>
-    <row r="29" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF28" s="31"/>
+    </row>
+    <row r="29" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="27"/>
       <c r="C29" s="29"/>
@@ -4265,8 +4314,9 @@
       <c r="BC29" s="29"/>
       <c r="BD29" s="29"/>
       <c r="BE29" s="30"/>
-    </row>
-    <row r="30" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF29" s="30"/>
+    </row>
+    <row r="30" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="25"/>
       <c r="C30" s="31"/>
@@ -4324,8 +4374,9 @@
       <c r="BC30" s="31"/>
       <c r="BD30" s="31"/>
       <c r="BE30" s="31"/>
-    </row>
-    <row r="31" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF30" s="31"/>
+    </row>
+    <row r="31" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="27"/>
       <c r="C31" s="29"/>
@@ -4383,8 +4434,9 @@
       <c r="BC31" s="29"/>
       <c r="BD31" s="29"/>
       <c r="BE31" s="30"/>
-    </row>
-    <row r="32" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF31" s="30"/>
+    </row>
+    <row r="32" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="25"/>
       <c r="C32" s="31"/>
@@ -4442,8 +4494,9 @@
       <c r="BC32" s="31"/>
       <c r="BD32" s="31"/>
       <c r="BE32" s="31"/>
-    </row>
-    <row r="33" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF32" s="31"/>
+    </row>
+    <row r="33" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="27"/>
       <c r="C33" s="29"/>
@@ -4501,8 +4554,9 @@
       <c r="BC33" s="29"/>
       <c r="BD33" s="29"/>
       <c r="BE33" s="30"/>
-    </row>
-    <row r="34" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF33" s="30"/>
+    </row>
+    <row r="34" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="25"/>
       <c r="C34" s="31"/>
@@ -4560,8 +4614,9 @@
       <c r="BC34" s="31"/>
       <c r="BD34" s="31"/>
       <c r="BE34" s="31"/>
-    </row>
-    <row r="35" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF34" s="31"/>
+    </row>
+    <row r="35" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="27"/>
       <c r="C35" s="29"/>
@@ -4619,8 +4674,9 @@
       <c r="BC35" s="29"/>
       <c r="BD35" s="29"/>
       <c r="BE35" s="30"/>
-    </row>
-    <row r="36" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF35" s="30"/>
+    </row>
+    <row r="36" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="25"/>
       <c r="C36" s="31"/>
@@ -4678,8 +4734,9 @@
       <c r="BC36" s="31"/>
       <c r="BD36" s="31"/>
       <c r="BE36" s="31"/>
-    </row>
-    <row r="37" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF36" s="31"/>
+    </row>
+    <row r="37" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="27"/>
       <c r="C37" s="29"/>
@@ -4737,8 +4794,9 @@
       <c r="BC37" s="29"/>
       <c r="BD37" s="29"/>
       <c r="BE37" s="30"/>
-    </row>
-    <row r="38" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF37" s="30"/>
+    </row>
+    <row r="38" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="25"/>
       <c r="C38" s="31"/>
@@ -4796,8 +4854,9 @@
       <c r="BC38" s="31"/>
       <c r="BD38" s="31"/>
       <c r="BE38" s="31"/>
-    </row>
-    <row r="39" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF38" s="31"/>
+    </row>
+    <row r="39" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="27"/>
       <c r="C39" s="29"/>
@@ -4855,8 +4914,9 @@
       <c r="BC39" s="29"/>
       <c r="BD39" s="29"/>
       <c r="BE39" s="30"/>
-    </row>
-    <row r="40" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF39" s="30"/>
+    </row>
+    <row r="40" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="25"/>
       <c r="C40" s="31"/>
@@ -4914,8 +4974,9 @@
       <c r="BC40" s="31"/>
       <c r="BD40" s="31"/>
       <c r="BE40" s="31"/>
-    </row>
-    <row r="41" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF40" s="31"/>
+    </row>
+    <row r="41" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="27"/>
       <c r="C41" s="29"/>
@@ -4973,8 +5034,9 @@
       <c r="BC41" s="29"/>
       <c r="BD41" s="29"/>
       <c r="BE41" s="30"/>
-    </row>
-    <row r="42" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF41" s="30"/>
+    </row>
+    <row r="42" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="25"/>
       <c r="C42" s="31"/>
@@ -5032,8 +5094,9 @@
       <c r="BC42" s="31"/>
       <c r="BD42" s="31"/>
       <c r="BE42" s="31"/>
-    </row>
-    <row r="43" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF42" s="31"/>
+    </row>
+    <row r="43" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="27"/>
       <c r="C43" s="29"/>
@@ -5091,8 +5154,9 @@
       <c r="BC43" s="29"/>
       <c r="BD43" s="29"/>
       <c r="BE43" s="30"/>
-    </row>
-    <row r="44" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF43" s="30"/>
+    </row>
+    <row r="44" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="25"/>
       <c r="C44" s="31"/>
@@ -5150,8 +5214,9 @@
       <c r="BC44" s="31"/>
       <c r="BD44" s="31"/>
       <c r="BE44" s="31"/>
-    </row>
-    <row r="45" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF44" s="31"/>
+    </row>
+    <row r="45" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="27"/>
       <c r="C45" s="29"/>
@@ -5209,8 +5274,9 @@
       <c r="BC45" s="29"/>
       <c r="BD45" s="29"/>
       <c r="BE45" s="30"/>
-    </row>
-    <row r="46" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF45" s="30"/>
+    </row>
+    <row r="46" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="25"/>
       <c r="C46" s="31"/>
@@ -5268,8 +5334,9 @@
       <c r="BC46" s="31"/>
       <c r="BD46" s="31"/>
       <c r="BE46" s="31"/>
-    </row>
-    <row r="47" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF46" s="31"/>
+    </row>
+    <row r="47" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="27"/>
       <c r="C47" s="29"/>
@@ -5327,8 +5394,9 @@
       <c r="BC47" s="29"/>
       <c r="BD47" s="29"/>
       <c r="BE47" s="30"/>
-    </row>
-    <row r="48" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF47" s="30"/>
+    </row>
+    <row r="48" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="25"/>
       <c r="C48" s="31"/>
@@ -5386,8 +5454,9 @@
       <c r="BC48" s="31"/>
       <c r="BD48" s="31"/>
       <c r="BE48" s="31"/>
-    </row>
-    <row r="49" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF48" s="31"/>
+    </row>
+    <row r="49" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="27"/>
       <c r="C49" s="29"/>
@@ -5445,8 +5514,9 @@
       <c r="BC49" s="29"/>
       <c r="BD49" s="29"/>
       <c r="BE49" s="30"/>
-    </row>
-    <row r="50" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF49" s="30"/>
+    </row>
+    <row r="50" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="32"/>
       <c r="B50" s="33"/>
       <c r="C50" s="34"/>
@@ -5504,11 +5574,13 @@
       <c r="BC50" s="34"/>
       <c r="BD50" s="34"/>
       <c r="BE50" s="34"/>
+      <c r="BF50" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:M1"/>
   </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
@@ -5533,10 +5605,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="80" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="69"/>
+      <c r="B1" s="81"/>
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -5626,8 +5698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV97"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5636,18 +5708,18 @@
     <col min="2" max="2" width="23.5" style="43" customWidth="1"/>
     <col min="3" max="3" width="11" style="43" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="43" customWidth="1"/>
-    <col min="5" max="5" width="23" style="65" customWidth="1"/>
+    <col min="5" max="5" width="23" style="64" customWidth="1"/>
     <col min="6" max="256" width="11" style="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
       <c r="F1" s="44"/>
       <c r="G1" s="44"/>
       <c r="H1" s="44"/>
@@ -5695,7 +5767,7 @@
       <c r="D3" s="52">
         <v>10</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="62">
         <v>50</v>
       </c>
       <c r="F3" s="37"/>
@@ -6810,10 +6882,14 @@
     </row>
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="59"/>
-      <c r="B59" s="60"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="64"/>
+      <c r="B59" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="86" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="87"/>
+      <c r="E59" s="87"/>
       <c r="F59" s="37"/>
       <c r="G59" s="37"/>
       <c r="H59" s="37"/>
@@ -6828,8 +6904,8 @@
       <c r="A60" s="59"/>
       <c r="B60" s="36"/>
       <c r="C60" s="37"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="64"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="63"/>
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
       <c r="H60" s="37"/>
@@ -6844,8 +6920,8 @@
       <c r="A61" s="59"/>
       <c r="B61" s="36"/>
       <c r="C61" s="37"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="64"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="63"/>
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
       <c r="H61" s="37"/>
@@ -6860,8 +6936,8 @@
       <c r="A62" s="59"/>
       <c r="B62" s="36"/>
       <c r="C62" s="37"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="64"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="63"/>
       <c r="F62" s="37"/>
       <c r="G62" s="37"/>
       <c r="H62" s="37"/>
@@ -6876,8 +6952,8 @@
       <c r="A63" s="59"/>
       <c r="B63" s="36"/>
       <c r="C63" s="37"/>
-      <c r="D63" s="61"/>
-      <c r="E63" s="64"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="63"/>
       <c r="F63" s="37"/>
       <c r="G63" s="37"/>
       <c r="H63" s="37"/>
@@ -6892,8 +6968,8 @@
       <c r="A64" s="59"/>
       <c r="B64" s="36"/>
       <c r="C64" s="37"/>
-      <c r="D64" s="61"/>
-      <c r="E64" s="64"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="63"/>
       <c r="F64" s="37"/>
       <c r="G64" s="37"/>
       <c r="H64" s="37"/>
@@ -6908,8 +6984,8 @@
       <c r="A65" s="59"/>
       <c r="B65" s="36"/>
       <c r="C65" s="37"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="64"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="63"/>
       <c r="F65" s="37"/>
       <c r="G65" s="37"/>
       <c r="H65" s="37"/>
@@ -6925,7 +7001,7 @@
       <c r="B66" s="36"/>
       <c r="C66" s="37"/>
       <c r="D66" s="56"/>
-      <c r="E66" s="64"/>
+      <c r="E66" s="63"/>
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
       <c r="H66" s="37"/>
@@ -6941,7 +7017,7 @@
       <c r="B67" s="36"/>
       <c r="C67" s="37"/>
       <c r="D67" s="56"/>
-      <c r="E67" s="64"/>
+      <c r="E67" s="63"/>
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
       <c r="H67" s="37"/>
@@ -6957,7 +7033,7 @@
       <c r="B68" s="36"/>
       <c r="C68" s="37"/>
       <c r="D68" s="56"/>
-      <c r="E68" s="64"/>
+      <c r="E68" s="63"/>
       <c r="F68" s="37"/>
       <c r="G68" s="37"/>
       <c r="H68" s="37"/>
@@ -6973,7 +7049,7 @@
       <c r="B69" s="36"/>
       <c r="C69" s="37"/>
       <c r="D69" s="56"/>
-      <c r="E69" s="64"/>
+      <c r="E69" s="63"/>
       <c r="F69" s="37"/>
       <c r="G69" s="37"/>
       <c r="H69" s="37"/>
@@ -6989,7 +7065,7 @@
       <c r="B70" s="36"/>
       <c r="C70" s="37"/>
       <c r="D70" s="56"/>
-      <c r="E70" s="64"/>
+      <c r="E70" s="63"/>
       <c r="F70" s="37"/>
       <c r="G70" s="37"/>
       <c r="H70" s="37"/>
@@ -7005,7 +7081,7 @@
       <c r="B71" s="36"/>
       <c r="C71" s="37"/>
       <c r="D71" s="56"/>
-      <c r="E71" s="64"/>
+      <c r="E71" s="63"/>
       <c r="F71" s="37"/>
       <c r="G71" s="37"/>
       <c r="H71" s="37"/>
@@ -7021,7 +7097,7 @@
       <c r="B72" s="36"/>
       <c r="C72" s="37"/>
       <c r="D72" s="56"/>
-      <c r="E72" s="64"/>
+      <c r="E72" s="63"/>
       <c r="F72" s="37"/>
       <c r="G72" s="37"/>
       <c r="H72" s="37"/>
@@ -7037,7 +7113,7 @@
       <c r="B73" s="36"/>
       <c r="C73" s="37"/>
       <c r="D73" s="56"/>
-      <c r="E73" s="64"/>
+      <c r="E73" s="63"/>
       <c r="F73" s="37"/>
       <c r="G73" s="37"/>
       <c r="H73" s="37"/>
@@ -7053,7 +7129,7 @@
       <c r="B74" s="36"/>
       <c r="C74" s="37"/>
       <c r="D74" s="56"/>
-      <c r="E74" s="64"/>
+      <c r="E74" s="63"/>
       <c r="F74" s="37"/>
       <c r="G74" s="37"/>
       <c r="H74" s="37"/>
@@ -7069,7 +7145,7 @@
       <c r="B75" s="36"/>
       <c r="C75" s="37"/>
       <c r="D75" s="56"/>
-      <c r="E75" s="64"/>
+      <c r="E75" s="63"/>
       <c r="F75" s="37"/>
       <c r="G75" s="37"/>
       <c r="H75" s="37"/>
@@ -7085,7 +7161,7 @@
       <c r="B76" s="36"/>
       <c r="C76" s="37"/>
       <c r="D76" s="56"/>
-      <c r="E76" s="64"/>
+      <c r="E76" s="63"/>
       <c r="F76" s="37"/>
       <c r="G76" s="37"/>
       <c r="H76" s="37"/>
@@ -7101,7 +7177,7 @@
       <c r="B77" s="36"/>
       <c r="C77" s="37"/>
       <c r="D77" s="56"/>
-      <c r="E77" s="64"/>
+      <c r="E77" s="63"/>
       <c r="F77" s="37"/>
       <c r="G77" s="37"/>
       <c r="H77" s="37"/>
@@ -7117,7 +7193,7 @@
       <c r="B78" s="36"/>
       <c r="C78" s="37"/>
       <c r="D78" s="56"/>
-      <c r="E78" s="64"/>
+      <c r="E78" s="63"/>
       <c r="F78" s="37"/>
       <c r="G78" s="37"/>
       <c r="H78" s="37"/>
@@ -7133,7 +7209,7 @@
       <c r="B79" s="36"/>
       <c r="C79" s="37"/>
       <c r="D79" s="56"/>
-      <c r="E79" s="64"/>
+      <c r="E79" s="63"/>
       <c r="F79" s="37"/>
       <c r="G79" s="37"/>
       <c r="H79" s="37"/>
@@ -7149,7 +7225,7 @@
       <c r="B80" s="36"/>
       <c r="C80" s="37"/>
       <c r="D80" s="56"/>
-      <c r="E80" s="64"/>
+      <c r="E80" s="63"/>
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
       <c r="H80" s="37"/>
@@ -7165,7 +7241,7 @@
       <c r="B81" s="36"/>
       <c r="C81" s="37"/>
       <c r="D81" s="56"/>
-      <c r="E81" s="64"/>
+      <c r="E81" s="63"/>
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
       <c r="H81" s="37"/>
@@ -7181,7 +7257,7 @@
       <c r="B82" s="36"/>
       <c r="C82" s="37"/>
       <c r="D82" s="56"/>
-      <c r="E82" s="64"/>
+      <c r="E82" s="63"/>
       <c r="F82" s="37"/>
       <c r="G82" s="37"/>
       <c r="H82" s="37"/>
@@ -7197,7 +7273,7 @@
       <c r="B83" s="36"/>
       <c r="C83" s="37"/>
       <c r="D83" s="56"/>
-      <c r="E83" s="64"/>
+      <c r="E83" s="63"/>
       <c r="F83" s="37"/>
       <c r="G83" s="37"/>
       <c r="H83" s="37"/>
@@ -7213,7 +7289,7 @@
       <c r="B84" s="36"/>
       <c r="C84" s="37"/>
       <c r="D84" s="56"/>
-      <c r="E84" s="64"/>
+      <c r="E84" s="63"/>
       <c r="F84" s="37"/>
       <c r="G84" s="37"/>
       <c r="H84" s="37"/>
@@ -7229,7 +7305,7 @@
       <c r="B85" s="36"/>
       <c r="C85" s="37"/>
       <c r="D85" s="56"/>
-      <c r="E85" s="64"/>
+      <c r="E85" s="63"/>
       <c r="F85" s="37"/>
       <c r="G85" s="37"/>
       <c r="H85" s="37"/>
@@ -7245,7 +7321,7 @@
       <c r="B86" s="36"/>
       <c r="C86" s="37"/>
       <c r="D86" s="56"/>
-      <c r="E86" s="64"/>
+      <c r="E86" s="63"/>
       <c r="F86" s="37"/>
       <c r="G86" s="37"/>
       <c r="H86" s="37"/>
@@ -7261,7 +7337,7 @@
       <c r="B87" s="36"/>
       <c r="C87" s="37"/>
       <c r="D87" s="56"/>
-      <c r="E87" s="64"/>
+      <c r="E87" s="63"/>
       <c r="F87" s="37"/>
       <c r="G87" s="37"/>
       <c r="H87" s="37"/>
@@ -7277,7 +7353,7 @@
       <c r="B88" s="36"/>
       <c r="C88" s="37"/>
       <c r="D88" s="56"/>
-      <c r="E88" s="64"/>
+      <c r="E88" s="63"/>
       <c r="F88" s="37"/>
       <c r="G88" s="37"/>
       <c r="H88" s="37"/>
@@ -7293,7 +7369,7 @@
       <c r="B89" s="36"/>
       <c r="C89" s="37"/>
       <c r="D89" s="56"/>
-      <c r="E89" s="64"/>
+      <c r="E89" s="63"/>
       <c r="F89" s="37"/>
       <c r="G89" s="37"/>
       <c r="H89" s="37"/>
@@ -7309,7 +7385,7 @@
       <c r="B90" s="36"/>
       <c r="C90" s="37"/>
       <c r="D90" s="56"/>
-      <c r="E90" s="64"/>
+      <c r="E90" s="63"/>
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
       <c r="H90" s="37"/>
@@ -7325,7 +7401,7 @@
       <c r="B91" s="36"/>
       <c r="C91" s="37"/>
       <c r="D91" s="56"/>
-      <c r="E91" s="64"/>
+      <c r="E91" s="63"/>
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
       <c r="H91" s="37"/>
@@ -7341,7 +7417,7 @@
       <c r="B92" s="36"/>
       <c r="C92" s="37"/>
       <c r="D92" s="56"/>
-      <c r="E92" s="64"/>
+      <c r="E92" s="63"/>
       <c r="F92" s="37"/>
       <c r="G92" s="37"/>
       <c r="H92" s="37"/>
@@ -7357,7 +7433,7 @@
       <c r="B93" s="36"/>
       <c r="C93" s="37"/>
       <c r="D93" s="56"/>
-      <c r="E93" s="64"/>
+      <c r="E93" s="63"/>
       <c r="F93" s="37"/>
       <c r="G93" s="37"/>
       <c r="H93" s="37"/>
@@ -7373,7 +7449,7 @@
       <c r="B94" s="36"/>
       <c r="C94" s="37"/>
       <c r="D94" s="56"/>
-      <c r="E94" s="64"/>
+      <c r="E94" s="63"/>
       <c r="F94" s="37"/>
       <c r="G94" s="37"/>
       <c r="H94" s="37"/>
@@ -7389,7 +7465,7 @@
       <c r="B95" s="36"/>
       <c r="C95" s="37"/>
       <c r="D95" s="56"/>
-      <c r="E95" s="64"/>
+      <c r="E95" s="63"/>
       <c r="F95" s="37"/>
       <c r="G95" s="37"/>
       <c r="H95" s="37"/>
@@ -7405,7 +7481,7 @@
       <c r="B96" s="36"/>
       <c r="C96" s="37"/>
       <c r="D96" s="56"/>
-      <c r="E96" s="64"/>
+      <c r="E96" s="63"/>
       <c r="F96" s="37"/>
       <c r="G96" s="37"/>
       <c r="H96" s="37"/>
@@ -7417,11 +7493,11 @@
       <c r="N96" s="37"/>
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="62"/>
+      <c r="A97" s="61"/>
       <c r="B97" s="36"/>
       <c r="C97" s="37"/>
       <c r="D97" s="56"/>
-      <c r="E97" s="64"/>
+      <c r="E97" s="63"/>
       <c r="F97" s="37"/>
       <c r="G97" s="37"/>
       <c r="H97" s="37"/>

</xml_diff>

<commit_message>
Added migration for allocation time slot details
</commit_message>
<xml_diff>
--- a/public/ROAssignmentTemplate.xlsx
+++ b/public/ROAssignmentTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1CBF7A-C1BD-B345-A313-3D37E92C1DDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A99A45-C137-214A-BD88-E23688619FD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="2460" windowWidth="19580" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5020" yWindow="1860" windowWidth="19580" windowHeight="14100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
   <si>
     <t>Example</t>
   </si>
@@ -384,26 +384,39 @@
     <t xml:space="preserve">Des Moines, IA </t>
   </si>
   <si>
-    <t>Number of Hearing Days Without Rooms in Date Range</t>
-  </si>
-  <si>
-    <t>Number of Hearing Days with 425 I Rooms Allocated in Date Range</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>NVHQ</t>
+  </si>
+  <si>
+    <t>Virtual Days</t>
+  </si>
+  <si>
+    <t># of Video Days</t>
+  </si>
+  <si>
+    <t># of Virtual Days</t>
+  </si>
+  <si>
+    <t>Number of Time Slots</t>
+  </si>
+  <si>
+    <t>Length of Time Slots (Minutes)</t>
+  </si>
+  <si>
+    <t>Start Time (Eastern)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -487,8 +500,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,8 +555,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -818,30 +842,6 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
@@ -930,19 +930,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -968,11 +955,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1060,31 +1089,31 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1095,6 +1124,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1107,18 +1139,34 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2311,7 +2359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IT50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="BB1" workbookViewId="0">
       <selection activeCell="BF4" sqref="BF4"/>
     </sheetView>
   </sheetViews>
@@ -2333,19 +2381,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2564,8 +2612,8 @@
       <c r="BE2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="BF2" s="86" t="s">
-        <v>123</v>
+      <c r="BF2" s="79" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:58" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -2740,8 +2788,8 @@
       <c r="BE3" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="BF3" s="85" t="s">
-        <v>122</v>
+      <c r="BF3" s="78" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:58" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -5605,10 +5653,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="84"/>
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -5696,10 +5744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV97"/>
+  <dimension ref="A1:IV98"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5713,16 +5761,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="87"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -5731,22 +5779,16 @@
       <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -5754,25 +5796,29 @@
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
     </row>
-    <row r="3" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="52">
-        <v>10</v>
-      </c>
-      <c r="E3" s="62">
-        <v>50</v>
-      </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+    <row r="3" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>127</v>
+      </c>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
@@ -5780,19 +5826,31 @@
       <c r="M3" s="37"/>
       <c r="N3" s="37"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+    <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="52">
+        <v>10</v>
+      </c>
+      <c r="E4" s="62">
+        <v>50</v>
+      </c>
+      <c r="F4" s="62">
+        <v>8</v>
+      </c>
+      <c r="G4" s="62">
+        <v>60</v>
+      </c>
+      <c r="H4" s="94">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="I4" s="37"/>
       <c r="J4" s="37"/>
       <c r="K4" s="37"/>
@@ -5801,12 +5859,12 @@
       <c r="N4" s="37"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
@@ -5821,12 +5879,12 @@
       <c r="N5" s="37"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="56"/>
       <c r="E6" s="56"/>
@@ -5841,12 +5899,12 @@
       <c r="N6" s="37"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="56"/>
       <c r="E7" s="56"/>
@@ -5863,10 +5921,10 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="59"/>
       <c r="B8" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="56"/>
       <c r="E8" s="56"/>
@@ -5883,10 +5941,10 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="59"/>
       <c r="B9" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="56"/>
       <c r="E9" s="56"/>
@@ -5903,10 +5961,10 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="B10" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="56"/>
       <c r="E10" s="56"/>
@@ -5923,10 +5981,10 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="B11" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="56"/>
@@ -5943,10 +6001,10 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="B12" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
@@ -5963,10 +6021,10 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="B13" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="56"/>
       <c r="E13" s="56"/>
@@ -5983,10 +6041,10 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="B14" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
@@ -6003,10 +6061,10 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="B15" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="56"/>
@@ -6023,10 +6081,10 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="59"/>
       <c r="B16" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
@@ -6043,10 +6101,10 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="59"/>
       <c r="B17" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
@@ -6063,10 +6121,10 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="59"/>
       <c r="B18" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
@@ -6083,10 +6141,10 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="59"/>
       <c r="B19" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
@@ -6103,10 +6161,10 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="59"/>
       <c r="B20" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
@@ -6123,10 +6181,10 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="59"/>
       <c r="B21" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
@@ -6143,10 +6201,10 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="59"/>
       <c r="B22" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
@@ -6163,10 +6221,10 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="59"/>
       <c r="B23" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
@@ -6183,10 +6241,10 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="59"/>
       <c r="B24" s="54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
@@ -6203,10 +6261,10 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="59"/>
       <c r="B25" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
@@ -6223,10 +6281,10 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="59"/>
       <c r="B26" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
@@ -6243,10 +6301,10 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="59"/>
       <c r="B27" s="54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
@@ -6263,10 +6321,10 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="59"/>
       <c r="B28" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
@@ -6283,10 +6341,10 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="59"/>
       <c r="B29" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
@@ -6303,10 +6361,10 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="59"/>
       <c r="B30" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="56"/>
       <c r="E30" s="56"/>
@@ -6323,10 +6381,10 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="59"/>
       <c r="B31" s="54" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C31" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="56"/>
       <c r="E31" s="56"/>
@@ -6343,10 +6401,10 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="59"/>
       <c r="B32" s="54" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
@@ -6363,10 +6421,10 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="59"/>
       <c r="B33" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="56"/>
       <c r="E33" s="56"/>
@@ -6383,10 +6441,10 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="59"/>
       <c r="B34" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
@@ -6403,10 +6461,10 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="59"/>
       <c r="B35" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="56"/>
       <c r="E35" s="56"/>
@@ -6423,10 +6481,10 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="59"/>
       <c r="B36" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
@@ -6443,10 +6501,10 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="59"/>
       <c r="B37" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D37" s="56"/>
       <c r="E37" s="56"/>
@@ -6463,10 +6521,10 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="59"/>
       <c r="B38" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D38" s="56"/>
       <c r="E38" s="56"/>
@@ -6483,10 +6541,10 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="59"/>
       <c r="B39" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
@@ -6503,10 +6561,10 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="59"/>
       <c r="B40" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
@@ -6523,10 +6581,10 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="59"/>
       <c r="B41" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
@@ -6543,10 +6601,10 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="59"/>
       <c r="B42" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
@@ -6563,10 +6621,10 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="59"/>
       <c r="B43" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
@@ -6583,10 +6641,10 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="59"/>
       <c r="B44" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C44" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
@@ -6603,10 +6661,10 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="59"/>
       <c r="B45" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="56"/>
       <c r="E45" s="56"/>
@@ -6623,10 +6681,10 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="59"/>
       <c r="B46" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
@@ -6643,10 +6701,10 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="59"/>
       <c r="B47" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" s="55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="56"/>
       <c r="E47" s="56"/>
@@ -6663,10 +6721,10 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="59"/>
       <c r="B48" s="54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
@@ -6683,10 +6741,10 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="59"/>
       <c r="B49" s="54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" s="55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="56"/>
       <c r="E49" s="56"/>
@@ -6703,10 +6761,10 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="59"/>
       <c r="B50" s="54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
@@ -6723,10 +6781,10 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="59"/>
       <c r="B51" s="54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C51" s="55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" s="56"/>
       <c r="E51" s="56"/>
@@ -6743,10 +6801,10 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="59"/>
       <c r="B52" s="54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52" s="55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" s="56"/>
       <c r="E52" s="56"/>
@@ -6763,10 +6821,10 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="59"/>
       <c r="B53" s="54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="56"/>
       <c r="E53" s="56"/>
@@ -6783,10 +6841,10 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="59"/>
       <c r="B54" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C54" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" s="56"/>
       <c r="E54" s="56"/>
@@ -6803,10 +6861,10 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="59"/>
       <c r="B55" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C55" s="55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="56"/>
       <c r="E55" s="56"/>
@@ -6823,10 +6881,10 @@
     <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="59"/>
       <c r="B56" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C56" s="55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="56"/>
       <c r="E56" s="56"/>
@@ -6843,10 +6901,10 @@
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="59"/>
       <c r="B57" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C57" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D57" s="56"/>
       <c r="E57" s="56"/>
@@ -6863,10 +6921,10 @@
     <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="59"/>
       <c r="B58" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C58" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D58" s="56"/>
       <c r="E58" s="56"/>
@@ -6882,14 +6940,14 @@
     </row>
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="59"/>
-      <c r="B59" s="85" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="86" t="s">
-        <v>123</v>
-      </c>
-      <c r="D59" s="87"/>
-      <c r="E59" s="87"/>
+      <c r="B59" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
       <c r="F59" s="37"/>
       <c r="G59" s="37"/>
       <c r="H59" s="37"/>
@@ -6902,10 +6960,14 @@
     </row>
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="59"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="63"/>
+      <c r="B60" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
       <c r="H60" s="37"/>
@@ -7000,7 +7062,7 @@
       <c r="A66" s="59"/>
       <c r="B66" s="36"/>
       <c r="C66" s="37"/>
-      <c r="D66" s="56"/>
+      <c r="D66" s="60"/>
       <c r="E66" s="63"/>
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
@@ -7493,7 +7555,7 @@
       <c r="N96" s="37"/>
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="61"/>
+      <c r="A97" s="59"/>
       <c r="B97" s="36"/>
       <c r="C97" s="37"/>
       <c r="D97" s="56"/>
@@ -7508,9 +7570,26 @@
       <c r="M97" s="37"/>
       <c r="N97" s="37"/>
     </row>
+    <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="61"/>
+      <c r="B98" s="36"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="56"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="37"/>
+      <c r="K98" s="37"/>
+      <c r="L98" s="37"/>
+      <c r="M98" s="37"/>
+      <c r="N98" s="37"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
CASEFLOW-4586 Add White River Junction to RO hearing template
</commit_message>
<xml_diff>
--- a/public/ROAssignmentTemplate.xlsx
+++ b/public/ROAssignmentTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyshields/git-repos/caseflow/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A99A45-C137-214A-BD88-E23688619FD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C352E0A2-8D2C-7540-8C05-406A4583FD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="1860" windowWidth="19580" windowHeight="14100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="130">
   <si>
     <t>Example</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Start Time (Eastern)</t>
+  </si>
+  <si>
+    <t>White River Junction, VT</t>
+  </si>
+  <si>
+    <t>RO05</t>
   </si>
 </sst>
 </file>
@@ -1127,6 +1133,16 @@
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,12 +1164,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,10 +1173,6 @@
     <xf numFmtId="49" fontId="14" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2357,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IT50"/>
+  <dimension ref="A1:IU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BF4" sqref="BF4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2370,31 +2376,32 @@
     <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="57" width="11" style="1" customWidth="1"/>
-    <col min="58" max="58" width="11" style="43" customWidth="1"/>
-    <col min="59" max="254" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="8" max="58" width="11" style="1" customWidth="1"/>
+    <col min="59" max="59" width="11" style="43" customWidth="1"/>
+    <col min="60" max="255" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="4"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -2437,10 +2444,11 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
-      <c r="BE1" s="5"/>
+      <c r="BE1" s="4"/>
       <c r="BF1" s="5"/>
-    </row>
-    <row r="2" spans="1:58" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:59" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2457,166 +2465,169 @@
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AI2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="9" t="s">
+      <c r="AJ2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="9" t="s">
+      <c r="AK2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="9" t="s">
+      <c r="AL2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AM2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AN2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AO2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AP2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="9" t="s">
+      <c r="AQ2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AR2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="9" t="s">
+      <c r="AS2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" s="9" t="s">
+      <c r="AT2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" s="9" t="s">
+      <c r="AU2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AU2" s="9" t="s">
+      <c r="AV2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AV2" s="9" t="s">
+      <c r="AW2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AW2" s="9" t="s">
+      <c r="AX2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AX2" s="9" t="s">
+      <c r="AY2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AY2" s="9" t="s">
+      <c r="AZ2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AZ2" s="9" t="s">
+      <c r="BA2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" s="9" t="s">
+      <c r="BB2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="BC2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BC2" s="9" t="s">
+      <c r="BD2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BD2" s="9" t="s">
+      <c r="BE2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BE2" s="9" t="s">
+      <c r="BF2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="BF2" s="79" t="s">
+      <c r="BG2" s="79" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:58" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2633,166 +2644,169 @@
         <v>63</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="U3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="V3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="W3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="X3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Z3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="AA3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AB3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AC3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AD3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AE3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AF3" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AG3" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AH3" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AI3" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AI3" s="12" t="s">
+      <c r="AJ3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AK3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AL3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AL3" s="12" t="s">
+      <c r="AM3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AM3" s="12" t="s">
+      <c r="AN3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AN3" s="12" t="s">
+      <c r="AO3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AO3" s="12" t="s">
+      <c r="AP3" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="AP3" s="12" t="s">
+      <c r="AQ3" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AQ3" s="12" t="s">
+      <c r="AR3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AR3" s="12" t="s">
+      <c r="AS3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AS3" s="12" t="s">
+      <c r="AT3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AT3" s="12" t="s">
+      <c r="AU3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="AU3" s="12" t="s">
+      <c r="AV3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AV3" s="12" t="s">
+      <c r="AW3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="AW3" s="12" t="s">
+      <c r="AX3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="AX3" s="12" t="s">
+      <c r="AY3" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="AY3" s="12" t="s">
+      <c r="AZ3" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="AZ3" s="12" t="s">
+      <c r="BA3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="BA3" s="12" t="s">
+      <c r="BB3" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="BB3" s="12" t="s">
+      <c r="BC3" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="BC3" s="12" t="s">
+      <c r="BD3" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="BD3" s="12" t="s">
+      <c r="BE3" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="BE3" s="12" t="s">
+      <c r="BF3" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="BF3" s="78" t="s">
+      <c r="BG3" s="78" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2855,8 +2869,9 @@
       <c r="BD4" s="67"/>
       <c r="BE4" s="67"/>
       <c r="BF4" s="67"/>
-    </row>
-    <row r="5" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG4" s="67"/>
+    </row>
+    <row r="5" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="18">
         <v>43497</v>
@@ -2915,10 +2930,11 @@
       <c r="BB5" s="70"/>
       <c r="BC5" s="70"/>
       <c r="BD5" s="70"/>
-      <c r="BE5" s="71"/>
+      <c r="BE5" s="70"/>
       <c r="BF5" s="71"/>
-    </row>
-    <row r="6" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG5" s="71"/>
+    </row>
+    <row r="6" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="20">
         <v>43540</v>
@@ -2979,8 +2995,9 @@
       <c r="BD6" s="74"/>
       <c r="BE6" s="74"/>
       <c r="BF6" s="74"/>
-    </row>
-    <row r="7" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG6" s="74"/>
+    </row>
+    <row r="7" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="21">
         <v>43576</v>
@@ -3039,10 +3056,11 @@
       <c r="BB7" s="70"/>
       <c r="BC7" s="70"/>
       <c r="BD7" s="70"/>
-      <c r="BE7" s="71"/>
+      <c r="BE7" s="70"/>
       <c r="BF7" s="71"/>
-    </row>
-    <row r="8" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG7" s="71"/>
+    </row>
+    <row r="8" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="23">
         <v>43604</v>
@@ -3103,8 +3121,9 @@
       <c r="BD8" s="74"/>
       <c r="BE8" s="74"/>
       <c r="BF8" s="74"/>
-    </row>
-    <row r="9" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG8" s="74"/>
+    </row>
+    <row r="9" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="77"/>
       <c r="C9" s="70"/>
@@ -3161,10 +3180,11 @@
       <c r="BB9" s="70"/>
       <c r="BC9" s="70"/>
       <c r="BD9" s="70"/>
-      <c r="BE9" s="71"/>
+      <c r="BE9" s="70"/>
       <c r="BF9" s="71"/>
-    </row>
-    <row r="10" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG9" s="71"/>
+    </row>
+    <row r="10" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="76"/>
       <c r="C10" s="74"/>
@@ -3223,8 +3243,9 @@
       <c r="BD10" s="74"/>
       <c r="BE10" s="74"/>
       <c r="BF10" s="74"/>
-    </row>
-    <row r="11" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG10" s="74"/>
+    </row>
+    <row r="11" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" s="27"/>
       <c r="C11" s="24"/>
@@ -3281,10 +3302,11 @@
       <c r="BB11" s="24"/>
       <c r="BC11" s="24"/>
       <c r="BD11" s="24"/>
-      <c r="BE11" s="28"/>
+      <c r="BE11" s="24"/>
       <c r="BF11" s="28"/>
-    </row>
-    <row r="12" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG11" s="28"/>
+    </row>
+    <row r="12" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
@@ -3343,8 +3365,9 @@
       <c r="BD12" s="26"/>
       <c r="BE12" s="26"/>
       <c r="BF12" s="26"/>
-    </row>
-    <row r="13" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG12" s="26"/>
+    </row>
+    <row r="13" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
       <c r="C13" s="29"/>
@@ -3401,10 +3424,11 @@
       <c r="BB13" s="29"/>
       <c r="BC13" s="29"/>
       <c r="BD13" s="29"/>
-      <c r="BE13" s="30"/>
+      <c r="BE13" s="29"/>
       <c r="BF13" s="30"/>
-    </row>
-    <row r="14" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG13" s="30"/>
+    </row>
+    <row r="14" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="25"/>
       <c r="C14" s="31"/>
@@ -3463,8 +3487,9 @@
       <c r="BD14" s="31"/>
       <c r="BE14" s="31"/>
       <c r="BF14" s="31"/>
-    </row>
-    <row r="15" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG14" s="31"/>
+    </row>
+    <row r="15" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
       <c r="C15" s="29"/>
@@ -3521,10 +3546,11 @@
       <c r="BB15" s="29"/>
       <c r="BC15" s="29"/>
       <c r="BD15" s="29"/>
-      <c r="BE15" s="30"/>
+      <c r="BE15" s="29"/>
       <c r="BF15" s="30"/>
-    </row>
-    <row r="16" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG15" s="30"/>
+    </row>
+    <row r="16" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="25"/>
       <c r="C16" s="31"/>
@@ -3583,8 +3609,9 @@
       <c r="BD16" s="31"/>
       <c r="BE16" s="31"/>
       <c r="BF16" s="31"/>
-    </row>
-    <row r="17" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG16" s="31"/>
+    </row>
+    <row r="17" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="27"/>
       <c r="C17" s="29"/>
@@ -3641,10 +3668,11 @@
       <c r="BB17" s="29"/>
       <c r="BC17" s="29"/>
       <c r="BD17" s="29"/>
-      <c r="BE17" s="30"/>
+      <c r="BE17" s="29"/>
       <c r="BF17" s="30"/>
-    </row>
-    <row r="18" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG17" s="30"/>
+    </row>
+    <row r="18" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="25"/>
       <c r="C18" s="31"/>
@@ -3703,8 +3731,9 @@
       <c r="BD18" s="31"/>
       <c r="BE18" s="31"/>
       <c r="BF18" s="31"/>
-    </row>
-    <row r="19" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG18" s="31"/>
+    </row>
+    <row r="19" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
       <c r="C19" s="29"/>
@@ -3761,10 +3790,11 @@
       <c r="BB19" s="29"/>
       <c r="BC19" s="29"/>
       <c r="BD19" s="29"/>
-      <c r="BE19" s="30"/>
+      <c r="BE19" s="29"/>
       <c r="BF19" s="30"/>
-    </row>
-    <row r="20" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG19" s="30"/>
+    </row>
+    <row r="20" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="25"/>
       <c r="C20" s="31"/>
@@ -3823,8 +3853,9 @@
       <c r="BD20" s="31"/>
       <c r="BE20" s="31"/>
       <c r="BF20" s="31"/>
-    </row>
-    <row r="21" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG20" s="31"/>
+    </row>
+    <row r="21" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="27"/>
       <c r="C21" s="29"/>
@@ -3881,10 +3912,11 @@
       <c r="BB21" s="29"/>
       <c r="BC21" s="29"/>
       <c r="BD21" s="29"/>
-      <c r="BE21" s="30"/>
+      <c r="BE21" s="29"/>
       <c r="BF21" s="30"/>
-    </row>
-    <row r="22" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG21" s="30"/>
+    </row>
+    <row r="22" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="25"/>
       <c r="C22" s="31"/>
@@ -3943,8 +3975,9 @@
       <c r="BD22" s="31"/>
       <c r="BE22" s="31"/>
       <c r="BF22" s="31"/>
-    </row>
-    <row r="23" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG22" s="31"/>
+    </row>
+    <row r="23" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="27"/>
       <c r="C23" s="29"/>
@@ -4001,10 +4034,11 @@
       <c r="BB23" s="29"/>
       <c r="BC23" s="29"/>
       <c r="BD23" s="29"/>
-      <c r="BE23" s="30"/>
+      <c r="BE23" s="29"/>
       <c r="BF23" s="30"/>
-    </row>
-    <row r="24" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG23" s="30"/>
+    </row>
+    <row r="24" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="25"/>
       <c r="C24" s="31"/>
@@ -4063,8 +4097,9 @@
       <c r="BD24" s="31"/>
       <c r="BE24" s="31"/>
       <c r="BF24" s="31"/>
-    </row>
-    <row r="25" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG24" s="31"/>
+    </row>
+    <row r="25" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="27"/>
       <c r="C25" s="29"/>
@@ -4121,10 +4156,11 @@
       <c r="BB25" s="29"/>
       <c r="BC25" s="29"/>
       <c r="BD25" s="29"/>
-      <c r="BE25" s="30"/>
+      <c r="BE25" s="29"/>
       <c r="BF25" s="30"/>
-    </row>
-    <row r="26" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG25" s="30"/>
+    </row>
+    <row r="26" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="25"/>
       <c r="C26" s="31"/>
@@ -4183,8 +4219,9 @@
       <c r="BD26" s="31"/>
       <c r="BE26" s="31"/>
       <c r="BF26" s="31"/>
-    </row>
-    <row r="27" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG26" s="31"/>
+    </row>
+    <row r="27" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="27"/>
       <c r="C27" s="29"/>
@@ -4241,10 +4278,11 @@
       <c r="BB27" s="29"/>
       <c r="BC27" s="29"/>
       <c r="BD27" s="29"/>
-      <c r="BE27" s="30"/>
+      <c r="BE27" s="29"/>
       <c r="BF27" s="30"/>
-    </row>
-    <row r="28" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG27" s="30"/>
+    </row>
+    <row r="28" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="25"/>
       <c r="C28" s="31"/>
@@ -4303,8 +4341,9 @@
       <c r="BD28" s="31"/>
       <c r="BE28" s="31"/>
       <c r="BF28" s="31"/>
-    </row>
-    <row r="29" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG28" s="31"/>
+    </row>
+    <row r="29" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="27"/>
       <c r="C29" s="29"/>
@@ -4361,10 +4400,11 @@
       <c r="BB29" s="29"/>
       <c r="BC29" s="29"/>
       <c r="BD29" s="29"/>
-      <c r="BE29" s="30"/>
+      <c r="BE29" s="29"/>
       <c r="BF29" s="30"/>
-    </row>
-    <row r="30" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG29" s="30"/>
+    </row>
+    <row r="30" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="25"/>
       <c r="C30" s="31"/>
@@ -4423,8 +4463,9 @@
       <c r="BD30" s="31"/>
       <c r="BE30" s="31"/>
       <c r="BF30" s="31"/>
-    </row>
-    <row r="31" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG30" s="31"/>
+    </row>
+    <row r="31" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="27"/>
       <c r="C31" s="29"/>
@@ -4481,10 +4522,11 @@
       <c r="BB31" s="29"/>
       <c r="BC31" s="29"/>
       <c r="BD31" s="29"/>
-      <c r="BE31" s="30"/>
+      <c r="BE31" s="29"/>
       <c r="BF31" s="30"/>
-    </row>
-    <row r="32" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG31" s="30"/>
+    </row>
+    <row r="32" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="25"/>
       <c r="C32" s="31"/>
@@ -4543,8 +4585,9 @@
       <c r="BD32" s="31"/>
       <c r="BE32" s="31"/>
       <c r="BF32" s="31"/>
-    </row>
-    <row r="33" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG32" s="31"/>
+    </row>
+    <row r="33" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="27"/>
       <c r="C33" s="29"/>
@@ -4601,10 +4644,11 @@
       <c r="BB33" s="29"/>
       <c r="BC33" s="29"/>
       <c r="BD33" s="29"/>
-      <c r="BE33" s="30"/>
+      <c r="BE33" s="29"/>
       <c r="BF33" s="30"/>
-    </row>
-    <row r="34" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG33" s="30"/>
+    </row>
+    <row r="34" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="25"/>
       <c r="C34" s="31"/>
@@ -4663,8 +4707,9 @@
       <c r="BD34" s="31"/>
       <c r="BE34" s="31"/>
       <c r="BF34" s="31"/>
-    </row>
-    <row r="35" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG34" s="31"/>
+    </row>
+    <row r="35" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="27"/>
       <c r="C35" s="29"/>
@@ -4721,10 +4766,11 @@
       <c r="BB35" s="29"/>
       <c r="BC35" s="29"/>
       <c r="BD35" s="29"/>
-      <c r="BE35" s="30"/>
+      <c r="BE35" s="29"/>
       <c r="BF35" s="30"/>
-    </row>
-    <row r="36" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG35" s="30"/>
+    </row>
+    <row r="36" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="25"/>
       <c r="C36" s="31"/>
@@ -4783,8 +4829,9 @@
       <c r="BD36" s="31"/>
       <c r="BE36" s="31"/>
       <c r="BF36" s="31"/>
-    </row>
-    <row r="37" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG36" s="31"/>
+    </row>
+    <row r="37" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="27"/>
       <c r="C37" s="29"/>
@@ -4841,10 +4888,11 @@
       <c r="BB37" s="29"/>
       <c r="BC37" s="29"/>
       <c r="BD37" s="29"/>
-      <c r="BE37" s="30"/>
+      <c r="BE37" s="29"/>
       <c r="BF37" s="30"/>
-    </row>
-    <row r="38" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG37" s="30"/>
+    </row>
+    <row r="38" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="25"/>
       <c r="C38" s="31"/>
@@ -4903,8 +4951,9 @@
       <c r="BD38" s="31"/>
       <c r="BE38" s="31"/>
       <c r="BF38" s="31"/>
-    </row>
-    <row r="39" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG38" s="31"/>
+    </row>
+    <row r="39" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="27"/>
       <c r="C39" s="29"/>
@@ -4961,10 +5010,11 @@
       <c r="BB39" s="29"/>
       <c r="BC39" s="29"/>
       <c r="BD39" s="29"/>
-      <c r="BE39" s="30"/>
+      <c r="BE39" s="29"/>
       <c r="BF39" s="30"/>
-    </row>
-    <row r="40" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG39" s="30"/>
+    </row>
+    <row r="40" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="25"/>
       <c r="C40" s="31"/>
@@ -5023,8 +5073,9 @@
       <c r="BD40" s="31"/>
       <c r="BE40" s="31"/>
       <c r="BF40" s="31"/>
-    </row>
-    <row r="41" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG40" s="31"/>
+    </row>
+    <row r="41" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="27"/>
       <c r="C41" s="29"/>
@@ -5081,10 +5132,11 @@
       <c r="BB41" s="29"/>
       <c r="BC41" s="29"/>
       <c r="BD41" s="29"/>
-      <c r="BE41" s="30"/>
+      <c r="BE41" s="29"/>
       <c r="BF41" s="30"/>
-    </row>
-    <row r="42" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG41" s="30"/>
+    </row>
+    <row r="42" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="25"/>
       <c r="C42" s="31"/>
@@ -5143,8 +5195,9 @@
       <c r="BD42" s="31"/>
       <c r="BE42" s="31"/>
       <c r="BF42" s="31"/>
-    </row>
-    <row r="43" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG42" s="31"/>
+    </row>
+    <row r="43" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="27"/>
       <c r="C43" s="29"/>
@@ -5201,10 +5254,11 @@
       <c r="BB43" s="29"/>
       <c r="BC43" s="29"/>
       <c r="BD43" s="29"/>
-      <c r="BE43" s="30"/>
+      <c r="BE43" s="29"/>
       <c r="BF43" s="30"/>
-    </row>
-    <row r="44" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG43" s="30"/>
+    </row>
+    <row r="44" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="25"/>
       <c r="C44" s="31"/>
@@ -5263,8 +5317,9 @@
       <c r="BD44" s="31"/>
       <c r="BE44" s="31"/>
       <c r="BF44" s="31"/>
-    </row>
-    <row r="45" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG44" s="31"/>
+    </row>
+    <row r="45" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="27"/>
       <c r="C45" s="29"/>
@@ -5321,10 +5376,11 @@
       <c r="BB45" s="29"/>
       <c r="BC45" s="29"/>
       <c r="BD45" s="29"/>
-      <c r="BE45" s="30"/>
+      <c r="BE45" s="29"/>
       <c r="BF45" s="30"/>
-    </row>
-    <row r="46" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG45" s="30"/>
+    </row>
+    <row r="46" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="25"/>
       <c r="C46" s="31"/>
@@ -5383,8 +5439,9 @@
       <c r="BD46" s="31"/>
       <c r="BE46" s="31"/>
       <c r="BF46" s="31"/>
-    </row>
-    <row r="47" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG46" s="31"/>
+    </row>
+    <row r="47" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="27"/>
       <c r="C47" s="29"/>
@@ -5441,10 +5498,11 @@
       <c r="BB47" s="29"/>
       <c r="BC47" s="29"/>
       <c r="BD47" s="29"/>
-      <c r="BE47" s="30"/>
+      <c r="BE47" s="29"/>
       <c r="BF47" s="30"/>
-    </row>
-    <row r="48" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG47" s="30"/>
+    </row>
+    <row r="48" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="25"/>
       <c r="C48" s="31"/>
@@ -5503,8 +5561,9 @@
       <c r="BD48" s="31"/>
       <c r="BE48" s="31"/>
       <c r="BF48" s="31"/>
-    </row>
-    <row r="49" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG48" s="31"/>
+    </row>
+    <row r="49" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="27"/>
       <c r="C49" s="29"/>
@@ -5561,10 +5620,11 @@
       <c r="BB49" s="29"/>
       <c r="BC49" s="29"/>
       <c r="BD49" s="29"/>
-      <c r="BE49" s="30"/>
+      <c r="BE49" s="29"/>
       <c r="BF49" s="30"/>
-    </row>
-    <row r="50" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG49" s="30"/>
+    </row>
+    <row r="50" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="32"/>
       <c r="B50" s="33"/>
       <c r="C50" s="34"/>
@@ -5623,10 +5683,11 @@
       <c r="BD50" s="34"/>
       <c r="BE50" s="34"/>
       <c r="BF50" s="34"/>
+      <c r="BG50" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5653,10 +5714,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="84"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -5744,10 +5805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV98"/>
+  <dimension ref="A1:IV99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5761,16 +5822,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="89" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="87"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -5779,16 +5840,16 @@
       <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90" t="s">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="92" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -5810,7 +5871,7 @@
       <c r="E3" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="83" t="s">
         <v>125</v>
       </c>
       <c r="G3" s="48" t="s">
@@ -5848,7 +5909,7 @@
       <c r="G4" s="62">
         <v>60</v>
       </c>
-      <c r="H4" s="94">
+      <c r="H4" s="84">
         <v>0.35416666666666669</v>
       </c>
       <c r="I4" s="37"/>
@@ -5921,10 +5982,10 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="59"/>
       <c r="B8" s="54" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="D8" s="56"/>
       <c r="E8" s="56"/>
@@ -5941,10 +6002,10 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="59"/>
       <c r="B9" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="56"/>
       <c r="E9" s="56"/>
@@ -5961,10 +6022,10 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="B10" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="56"/>
       <c r="E10" s="56"/>
@@ -5981,10 +6042,10 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="B11" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="56"/>
@@ -6001,10 +6062,10 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="B12" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
@@ -6021,10 +6082,10 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="B13" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="56"/>
       <c r="E13" s="56"/>
@@ -6041,10 +6102,10 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="B14" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
@@ -6061,10 +6122,10 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="B15" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="56"/>
@@ -6081,10 +6142,10 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="59"/>
       <c r="B16" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
@@ -6101,10 +6162,10 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="59"/>
       <c r="B17" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
@@ -6121,10 +6182,10 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="59"/>
       <c r="B18" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
@@ -6141,10 +6202,10 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="59"/>
       <c r="B19" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
@@ -6161,10 +6222,10 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="59"/>
       <c r="B20" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
@@ -6181,10 +6242,10 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="59"/>
       <c r="B21" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
@@ -6201,10 +6262,10 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="59"/>
       <c r="B22" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
@@ -6221,10 +6282,10 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="59"/>
       <c r="B23" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
@@ -6241,10 +6302,10 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="59"/>
       <c r="B24" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
@@ -6261,10 +6322,10 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="59"/>
       <c r="B25" s="54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
@@ -6281,10 +6342,10 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="59"/>
       <c r="B26" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
@@ -6301,10 +6362,10 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="59"/>
       <c r="B27" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
@@ -6321,10 +6382,10 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="59"/>
       <c r="B28" s="54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
@@ -6341,10 +6402,10 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="59"/>
       <c r="B29" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
@@ -6361,10 +6422,10 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="59"/>
       <c r="B30" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="56"/>
       <c r="E30" s="56"/>
@@ -6381,10 +6442,10 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="59"/>
       <c r="B31" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="55" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="56"/>
       <c r="E31" s="56"/>
@@ -6401,10 +6462,10 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="59"/>
       <c r="B32" s="54" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
@@ -6421,10 +6482,10 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="59"/>
       <c r="B33" s="54" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="56"/>
       <c r="E33" s="56"/>
@@ -6441,10 +6502,10 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="59"/>
       <c r="B34" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
@@ -6461,10 +6522,10 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="59"/>
       <c r="B35" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="56"/>
       <c r="E35" s="56"/>
@@ -6481,10 +6542,10 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="59"/>
       <c r="B36" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
@@ -6501,10 +6562,10 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="59"/>
       <c r="B37" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="56"/>
       <c r="E37" s="56"/>
@@ -6521,10 +6582,10 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="59"/>
       <c r="B38" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="56"/>
       <c r="E38" s="56"/>
@@ -6541,10 +6602,10 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="59"/>
       <c r="B39" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
@@ -6561,10 +6622,10 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="59"/>
       <c r="B40" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
@@ -6581,10 +6642,10 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="59"/>
       <c r="B41" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
@@ -6601,10 +6662,10 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="59"/>
       <c r="B42" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
@@ -6621,10 +6682,10 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="59"/>
       <c r="B43" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
@@ -6641,10 +6702,10 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="59"/>
       <c r="B44" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
@@ -6661,10 +6722,10 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="59"/>
       <c r="B45" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="56"/>
       <c r="E45" s="56"/>
@@ -6681,10 +6742,10 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="59"/>
       <c r="B46" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
@@ -6701,10 +6762,10 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="59"/>
       <c r="B47" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" s="56"/>
       <c r="E47" s="56"/>
@@ -6721,10 +6782,10 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="59"/>
       <c r="B48" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" s="55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
@@ -6741,10 +6802,10 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="59"/>
       <c r="B49" s="54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" s="56"/>
       <c r="E49" s="56"/>
@@ -6761,10 +6822,10 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="59"/>
       <c r="B50" s="54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
@@ -6781,10 +6842,10 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="59"/>
       <c r="B51" s="54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" s="55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" s="56"/>
       <c r="E51" s="56"/>
@@ -6801,10 +6862,10 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="59"/>
       <c r="B52" s="54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" s="55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="56"/>
       <c r="E52" s="56"/>
@@ -6821,10 +6882,10 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="59"/>
       <c r="B53" s="54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53" s="56"/>
       <c r="E53" s="56"/>
@@ -6841,10 +6902,10 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="59"/>
       <c r="B54" s="54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" s="55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" s="56"/>
       <c r="E54" s="56"/>
@@ -6861,10 +6922,10 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="59"/>
       <c r="B55" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D55" s="56"/>
       <c r="E55" s="56"/>
@@ -6881,10 +6942,10 @@
     <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="59"/>
       <c r="B56" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" s="55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="56"/>
       <c r="E56" s="56"/>
@@ -6901,10 +6962,10 @@
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="59"/>
       <c r="B57" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" s="55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" s="56"/>
       <c r="E57" s="56"/>
@@ -6921,10 +6982,10 @@
     <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="59"/>
       <c r="B58" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="56"/>
       <c r="E58" s="56"/>
@@ -6941,10 +7002,10 @@
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="59"/>
       <c r="B59" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="56"/>
       <c r="E59" s="56"/>
@@ -6960,14 +7021,14 @@
     </row>
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="59"/>
-      <c r="B60" s="78" t="s">
-        <v>120</v>
-      </c>
-      <c r="C60" s="79" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" s="80"/>
-      <c r="E60" s="80"/>
+      <c r="B60" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
       <c r="H60" s="37"/>
@@ -6980,10 +7041,14 @@
     </row>
     <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="59"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="63"/>
+      <c r="B61" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" s="80"/>
+      <c r="E61" s="80"/>
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
       <c r="H61" s="37"/>
@@ -7078,7 +7143,7 @@
       <c r="A67" s="59"/>
       <c r="B67" s="36"/>
       <c r="C67" s="37"/>
-      <c r="D67" s="56"/>
+      <c r="D67" s="60"/>
       <c r="E67" s="63"/>
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
@@ -7571,7 +7636,7 @@
       <c r="N97" s="37"/>
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="61"/>
+      <c r="A98" s="59"/>
       <c r="B98" s="36"/>
       <c r="C98" s="37"/>
       <c r="D98" s="56"/>
@@ -7586,6 +7651,22 @@
       <c r="M98" s="37"/>
       <c r="N98" s="37"/>
     </row>
+    <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="61"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="63"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
+      <c r="K99" s="37"/>
+      <c r="L99" s="37"/>
+      <c r="M99" s="37"/>
+      <c r="N99" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>

</xml_diff>

<commit_message>
Hotfix/merge branch 4575 4586 (#17194)
CASEFLOW-45756 and CASEFLOW-4586
</commit_message>
<xml_diff>
--- a/public/ROAssignmentTemplate.xlsx
+++ b/public/ROAssignmentTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyshields/git-repos/caseflow/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A99A45-C137-214A-BD88-E23688619FD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C352E0A2-8D2C-7540-8C05-406A4583FD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="1860" windowWidth="19580" windowHeight="14100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="130">
   <si>
     <t>Example</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Start Time (Eastern)</t>
+  </si>
+  <si>
+    <t>White River Junction, VT</t>
+  </si>
+  <si>
+    <t>RO05</t>
   </si>
 </sst>
 </file>
@@ -1127,6 +1133,16 @@
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,12 +1164,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,10 +1173,6 @@
     <xf numFmtId="49" fontId="14" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2357,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IT50"/>
+  <dimension ref="A1:IU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BF4" sqref="BF4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2370,31 +2376,32 @@
     <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="57" width="11" style="1" customWidth="1"/>
-    <col min="58" max="58" width="11" style="43" customWidth="1"/>
-    <col min="59" max="254" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="8" max="58" width="11" style="1" customWidth="1"/>
+    <col min="59" max="59" width="11" style="43" customWidth="1"/>
+    <col min="60" max="255" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="4"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -2437,10 +2444,11 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
-      <c r="BE1" s="5"/>
+      <c r="BE1" s="4"/>
       <c r="BF1" s="5"/>
-    </row>
-    <row r="2" spans="1:58" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:59" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2457,166 +2465,169 @@
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AI2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="9" t="s">
+      <c r="AJ2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="9" t="s">
+      <c r="AK2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="9" t="s">
+      <c r="AL2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AM2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AN2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AO2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AP2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="9" t="s">
+      <c r="AQ2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AR2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="9" t="s">
+      <c r="AS2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" s="9" t="s">
+      <c r="AT2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" s="9" t="s">
+      <c r="AU2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AU2" s="9" t="s">
+      <c r="AV2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AV2" s="9" t="s">
+      <c r="AW2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AW2" s="9" t="s">
+      <c r="AX2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AX2" s="9" t="s">
+      <c r="AY2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AY2" s="9" t="s">
+      <c r="AZ2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AZ2" s="9" t="s">
+      <c r="BA2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" s="9" t="s">
+      <c r="BB2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="BC2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BC2" s="9" t="s">
+      <c r="BD2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BD2" s="9" t="s">
+      <c r="BE2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BE2" s="9" t="s">
+      <c r="BF2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="BF2" s="79" t="s">
+      <c r="BG2" s="79" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:58" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2633,166 +2644,169 @@
         <v>63</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="U3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="V3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="W3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="X3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Z3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="AA3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AB3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AC3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AD3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AE3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AF3" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AG3" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AH3" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AI3" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AI3" s="12" t="s">
+      <c r="AJ3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AK3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AL3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AL3" s="12" t="s">
+      <c r="AM3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AM3" s="12" t="s">
+      <c r="AN3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AN3" s="12" t="s">
+      <c r="AO3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AO3" s="12" t="s">
+      <c r="AP3" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="AP3" s="12" t="s">
+      <c r="AQ3" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AQ3" s="12" t="s">
+      <c r="AR3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AR3" s="12" t="s">
+      <c r="AS3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AS3" s="12" t="s">
+      <c r="AT3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AT3" s="12" t="s">
+      <c r="AU3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="AU3" s="12" t="s">
+      <c r="AV3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AV3" s="12" t="s">
+      <c r="AW3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="AW3" s="12" t="s">
+      <c r="AX3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="AX3" s="12" t="s">
+      <c r="AY3" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="AY3" s="12" t="s">
+      <c r="AZ3" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="AZ3" s="12" t="s">
+      <c r="BA3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="BA3" s="12" t="s">
+      <c r="BB3" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="BB3" s="12" t="s">
+      <c r="BC3" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="BC3" s="12" t="s">
+      <c r="BD3" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="BD3" s="12" t="s">
+      <c r="BE3" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="BE3" s="12" t="s">
+      <c r="BF3" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="BF3" s="78" t="s">
+      <c r="BG3" s="78" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2855,8 +2869,9 @@
       <c r="BD4" s="67"/>
       <c r="BE4" s="67"/>
       <c r="BF4" s="67"/>
-    </row>
-    <row r="5" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG4" s="67"/>
+    </row>
+    <row r="5" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="18">
         <v>43497</v>
@@ -2915,10 +2930,11 @@
       <c r="BB5" s="70"/>
       <c r="BC5" s="70"/>
       <c r="BD5" s="70"/>
-      <c r="BE5" s="71"/>
+      <c r="BE5" s="70"/>
       <c r="BF5" s="71"/>
-    </row>
-    <row r="6" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG5" s="71"/>
+    </row>
+    <row r="6" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="20">
         <v>43540</v>
@@ -2979,8 +2995,9 @@
       <c r="BD6" s="74"/>
       <c r="BE6" s="74"/>
       <c r="BF6" s="74"/>
-    </row>
-    <row r="7" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG6" s="74"/>
+    </row>
+    <row r="7" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="21">
         <v>43576</v>
@@ -3039,10 +3056,11 @@
       <c r="BB7" s="70"/>
       <c r="BC7" s="70"/>
       <c r="BD7" s="70"/>
-      <c r="BE7" s="71"/>
+      <c r="BE7" s="70"/>
       <c r="BF7" s="71"/>
-    </row>
-    <row r="8" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG7" s="71"/>
+    </row>
+    <row r="8" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="23">
         <v>43604</v>
@@ -3103,8 +3121,9 @@
       <c r="BD8" s="74"/>
       <c r="BE8" s="74"/>
       <c r="BF8" s="74"/>
-    </row>
-    <row r="9" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG8" s="74"/>
+    </row>
+    <row r="9" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="77"/>
       <c r="C9" s="70"/>
@@ -3161,10 +3180,11 @@
       <c r="BB9" s="70"/>
       <c r="BC9" s="70"/>
       <c r="BD9" s="70"/>
-      <c r="BE9" s="71"/>
+      <c r="BE9" s="70"/>
       <c r="BF9" s="71"/>
-    </row>
-    <row r="10" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG9" s="71"/>
+    </row>
+    <row r="10" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="76"/>
       <c r="C10" s="74"/>
@@ -3223,8 +3243,9 @@
       <c r="BD10" s="74"/>
       <c r="BE10" s="74"/>
       <c r="BF10" s="74"/>
-    </row>
-    <row r="11" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG10" s="74"/>
+    </row>
+    <row r="11" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" s="27"/>
       <c r="C11" s="24"/>
@@ -3281,10 +3302,11 @@
       <c r="BB11" s="24"/>
       <c r="BC11" s="24"/>
       <c r="BD11" s="24"/>
-      <c r="BE11" s="28"/>
+      <c r="BE11" s="24"/>
       <c r="BF11" s="28"/>
-    </row>
-    <row r="12" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG11" s="28"/>
+    </row>
+    <row r="12" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
@@ -3343,8 +3365,9 @@
       <c r="BD12" s="26"/>
       <c r="BE12" s="26"/>
       <c r="BF12" s="26"/>
-    </row>
-    <row r="13" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG12" s="26"/>
+    </row>
+    <row r="13" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
       <c r="C13" s="29"/>
@@ -3401,10 +3424,11 @@
       <c r="BB13" s="29"/>
       <c r="BC13" s="29"/>
       <c r="BD13" s="29"/>
-      <c r="BE13" s="30"/>
+      <c r="BE13" s="29"/>
       <c r="BF13" s="30"/>
-    </row>
-    <row r="14" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG13" s="30"/>
+    </row>
+    <row r="14" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="25"/>
       <c r="C14" s="31"/>
@@ -3463,8 +3487,9 @@
       <c r="BD14" s="31"/>
       <c r="BE14" s="31"/>
       <c r="BF14" s="31"/>
-    </row>
-    <row r="15" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG14" s="31"/>
+    </row>
+    <row r="15" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
       <c r="C15" s="29"/>
@@ -3521,10 +3546,11 @@
       <c r="BB15" s="29"/>
       <c r="BC15" s="29"/>
       <c r="BD15" s="29"/>
-      <c r="BE15" s="30"/>
+      <c r="BE15" s="29"/>
       <c r="BF15" s="30"/>
-    </row>
-    <row r="16" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG15" s="30"/>
+    </row>
+    <row r="16" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="25"/>
       <c r="C16" s="31"/>
@@ -3583,8 +3609,9 @@
       <c r="BD16" s="31"/>
       <c r="BE16" s="31"/>
       <c r="BF16" s="31"/>
-    </row>
-    <row r="17" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG16" s="31"/>
+    </row>
+    <row r="17" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="27"/>
       <c r="C17" s="29"/>
@@ -3641,10 +3668,11 @@
       <c r="BB17" s="29"/>
       <c r="BC17" s="29"/>
       <c r="BD17" s="29"/>
-      <c r="BE17" s="30"/>
+      <c r="BE17" s="29"/>
       <c r="BF17" s="30"/>
-    </row>
-    <row r="18" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG17" s="30"/>
+    </row>
+    <row r="18" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="25"/>
       <c r="C18" s="31"/>
@@ -3703,8 +3731,9 @@
       <c r="BD18" s="31"/>
       <c r="BE18" s="31"/>
       <c r="BF18" s="31"/>
-    </row>
-    <row r="19" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG18" s="31"/>
+    </row>
+    <row r="19" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
       <c r="C19" s="29"/>
@@ -3761,10 +3790,11 @@
       <c r="BB19" s="29"/>
       <c r="BC19" s="29"/>
       <c r="BD19" s="29"/>
-      <c r="BE19" s="30"/>
+      <c r="BE19" s="29"/>
       <c r="BF19" s="30"/>
-    </row>
-    <row r="20" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG19" s="30"/>
+    </row>
+    <row r="20" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="25"/>
       <c r="C20" s="31"/>
@@ -3823,8 +3853,9 @@
       <c r="BD20" s="31"/>
       <c r="BE20" s="31"/>
       <c r="BF20" s="31"/>
-    </row>
-    <row r="21" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG20" s="31"/>
+    </row>
+    <row r="21" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="27"/>
       <c r="C21" s="29"/>
@@ -3881,10 +3912,11 @@
       <c r="BB21" s="29"/>
       <c r="BC21" s="29"/>
       <c r="BD21" s="29"/>
-      <c r="BE21" s="30"/>
+      <c r="BE21" s="29"/>
       <c r="BF21" s="30"/>
-    </row>
-    <row r="22" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG21" s="30"/>
+    </row>
+    <row r="22" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="25"/>
       <c r="C22" s="31"/>
@@ -3943,8 +3975,9 @@
       <c r="BD22" s="31"/>
       <c r="BE22" s="31"/>
       <c r="BF22" s="31"/>
-    </row>
-    <row r="23" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG22" s="31"/>
+    </row>
+    <row r="23" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="27"/>
       <c r="C23" s="29"/>
@@ -4001,10 +4034,11 @@
       <c r="BB23" s="29"/>
       <c r="BC23" s="29"/>
       <c r="BD23" s="29"/>
-      <c r="BE23" s="30"/>
+      <c r="BE23" s="29"/>
       <c r="BF23" s="30"/>
-    </row>
-    <row r="24" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG23" s="30"/>
+    </row>
+    <row r="24" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="25"/>
       <c r="C24" s="31"/>
@@ -4063,8 +4097,9 @@
       <c r="BD24" s="31"/>
       <c r="BE24" s="31"/>
       <c r="BF24" s="31"/>
-    </row>
-    <row r="25" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG24" s="31"/>
+    </row>
+    <row r="25" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="27"/>
       <c r="C25" s="29"/>
@@ -4121,10 +4156,11 @@
       <c r="BB25" s="29"/>
       <c r="BC25" s="29"/>
       <c r="BD25" s="29"/>
-      <c r="BE25" s="30"/>
+      <c r="BE25" s="29"/>
       <c r="BF25" s="30"/>
-    </row>
-    <row r="26" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG25" s="30"/>
+    </row>
+    <row r="26" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="25"/>
       <c r="C26" s="31"/>
@@ -4183,8 +4219,9 @@
       <c r="BD26" s="31"/>
       <c r="BE26" s="31"/>
       <c r="BF26" s="31"/>
-    </row>
-    <row r="27" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG26" s="31"/>
+    </row>
+    <row r="27" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="27"/>
       <c r="C27" s="29"/>
@@ -4241,10 +4278,11 @@
       <c r="BB27" s="29"/>
       <c r="BC27" s="29"/>
       <c r="BD27" s="29"/>
-      <c r="BE27" s="30"/>
+      <c r="BE27" s="29"/>
       <c r="BF27" s="30"/>
-    </row>
-    <row r="28" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG27" s="30"/>
+    </row>
+    <row r="28" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="25"/>
       <c r="C28" s="31"/>
@@ -4303,8 +4341,9 @@
       <c r="BD28" s="31"/>
       <c r="BE28" s="31"/>
       <c r="BF28" s="31"/>
-    </row>
-    <row r="29" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG28" s="31"/>
+    </row>
+    <row r="29" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="27"/>
       <c r="C29" s="29"/>
@@ -4361,10 +4400,11 @@
       <c r="BB29" s="29"/>
       <c r="BC29" s="29"/>
       <c r="BD29" s="29"/>
-      <c r="BE29" s="30"/>
+      <c r="BE29" s="29"/>
       <c r="BF29" s="30"/>
-    </row>
-    <row r="30" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG29" s="30"/>
+    </row>
+    <row r="30" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="25"/>
       <c r="C30" s="31"/>
@@ -4423,8 +4463,9 @@
       <c r="BD30" s="31"/>
       <c r="BE30" s="31"/>
       <c r="BF30" s="31"/>
-    </row>
-    <row r="31" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG30" s="31"/>
+    </row>
+    <row r="31" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="27"/>
       <c r="C31" s="29"/>
@@ -4481,10 +4522,11 @@
       <c r="BB31" s="29"/>
       <c r="BC31" s="29"/>
       <c r="BD31" s="29"/>
-      <c r="BE31" s="30"/>
+      <c r="BE31" s="29"/>
       <c r="BF31" s="30"/>
-    </row>
-    <row r="32" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG31" s="30"/>
+    </row>
+    <row r="32" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="25"/>
       <c r="C32" s="31"/>
@@ -4543,8 +4585,9 @@
       <c r="BD32" s="31"/>
       <c r="BE32" s="31"/>
       <c r="BF32" s="31"/>
-    </row>
-    <row r="33" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG32" s="31"/>
+    </row>
+    <row r="33" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="27"/>
       <c r="C33" s="29"/>
@@ -4601,10 +4644,11 @@
       <c r="BB33" s="29"/>
       <c r="BC33" s="29"/>
       <c r="BD33" s="29"/>
-      <c r="BE33" s="30"/>
+      <c r="BE33" s="29"/>
       <c r="BF33" s="30"/>
-    </row>
-    <row r="34" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG33" s="30"/>
+    </row>
+    <row r="34" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="25"/>
       <c r="C34" s="31"/>
@@ -4663,8 +4707,9 @@
       <c r="BD34" s="31"/>
       <c r="BE34" s="31"/>
       <c r="BF34" s="31"/>
-    </row>
-    <row r="35" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG34" s="31"/>
+    </row>
+    <row r="35" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="27"/>
       <c r="C35" s="29"/>
@@ -4721,10 +4766,11 @@
       <c r="BB35" s="29"/>
       <c r="BC35" s="29"/>
       <c r="BD35" s="29"/>
-      <c r="BE35" s="30"/>
+      <c r="BE35" s="29"/>
       <c r="BF35" s="30"/>
-    </row>
-    <row r="36" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG35" s="30"/>
+    </row>
+    <row r="36" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="25"/>
       <c r="C36" s="31"/>
@@ -4783,8 +4829,9 @@
       <c r="BD36" s="31"/>
       <c r="BE36" s="31"/>
       <c r="BF36" s="31"/>
-    </row>
-    <row r="37" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG36" s="31"/>
+    </row>
+    <row r="37" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="27"/>
       <c r="C37" s="29"/>
@@ -4841,10 +4888,11 @@
       <c r="BB37" s="29"/>
       <c r="BC37" s="29"/>
       <c r="BD37" s="29"/>
-      <c r="BE37" s="30"/>
+      <c r="BE37" s="29"/>
       <c r="BF37" s="30"/>
-    </row>
-    <row r="38" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG37" s="30"/>
+    </row>
+    <row r="38" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="25"/>
       <c r="C38" s="31"/>
@@ -4903,8 +4951,9 @@
       <c r="BD38" s="31"/>
       <c r="BE38" s="31"/>
       <c r="BF38" s="31"/>
-    </row>
-    <row r="39" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG38" s="31"/>
+    </row>
+    <row r="39" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="27"/>
       <c r="C39" s="29"/>
@@ -4961,10 +5010,11 @@
       <c r="BB39" s="29"/>
       <c r="BC39" s="29"/>
       <c r="BD39" s="29"/>
-      <c r="BE39" s="30"/>
+      <c r="BE39" s="29"/>
       <c r="BF39" s="30"/>
-    </row>
-    <row r="40" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG39" s="30"/>
+    </row>
+    <row r="40" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="25"/>
       <c r="C40" s="31"/>
@@ -5023,8 +5073,9 @@
       <c r="BD40" s="31"/>
       <c r="BE40" s="31"/>
       <c r="BF40" s="31"/>
-    </row>
-    <row r="41" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG40" s="31"/>
+    </row>
+    <row r="41" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="27"/>
       <c r="C41" s="29"/>
@@ -5081,10 +5132,11 @@
       <c r="BB41" s="29"/>
       <c r="BC41" s="29"/>
       <c r="BD41" s="29"/>
-      <c r="BE41" s="30"/>
+      <c r="BE41" s="29"/>
       <c r="BF41" s="30"/>
-    </row>
-    <row r="42" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG41" s="30"/>
+    </row>
+    <row r="42" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="25"/>
       <c r="C42" s="31"/>
@@ -5143,8 +5195,9 @@
       <c r="BD42" s="31"/>
       <c r="BE42" s="31"/>
       <c r="BF42" s="31"/>
-    </row>
-    <row r="43" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG42" s="31"/>
+    </row>
+    <row r="43" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="27"/>
       <c r="C43" s="29"/>
@@ -5201,10 +5254,11 @@
       <c r="BB43" s="29"/>
       <c r="BC43" s="29"/>
       <c r="BD43" s="29"/>
-      <c r="BE43" s="30"/>
+      <c r="BE43" s="29"/>
       <c r="BF43" s="30"/>
-    </row>
-    <row r="44" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG43" s="30"/>
+    </row>
+    <row r="44" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="25"/>
       <c r="C44" s="31"/>
@@ -5263,8 +5317,9 @@
       <c r="BD44" s="31"/>
       <c r="BE44" s="31"/>
       <c r="BF44" s="31"/>
-    </row>
-    <row r="45" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG44" s="31"/>
+    </row>
+    <row r="45" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="27"/>
       <c r="C45" s="29"/>
@@ -5321,10 +5376,11 @@
       <c r="BB45" s="29"/>
       <c r="BC45" s="29"/>
       <c r="BD45" s="29"/>
-      <c r="BE45" s="30"/>
+      <c r="BE45" s="29"/>
       <c r="BF45" s="30"/>
-    </row>
-    <row r="46" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG45" s="30"/>
+    </row>
+    <row r="46" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="25"/>
       <c r="C46" s="31"/>
@@ -5383,8 +5439,9 @@
       <c r="BD46" s="31"/>
       <c r="BE46" s="31"/>
       <c r="BF46" s="31"/>
-    </row>
-    <row r="47" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG46" s="31"/>
+    </row>
+    <row r="47" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="27"/>
       <c r="C47" s="29"/>
@@ -5441,10 +5498,11 @@
       <c r="BB47" s="29"/>
       <c r="BC47" s="29"/>
       <c r="BD47" s="29"/>
-      <c r="BE47" s="30"/>
+      <c r="BE47" s="29"/>
       <c r="BF47" s="30"/>
-    </row>
-    <row r="48" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG47" s="30"/>
+    </row>
+    <row r="48" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="25"/>
       <c r="C48" s="31"/>
@@ -5503,8 +5561,9 @@
       <c r="BD48" s="31"/>
       <c r="BE48" s="31"/>
       <c r="BF48" s="31"/>
-    </row>
-    <row r="49" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG48" s="31"/>
+    </row>
+    <row r="49" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="27"/>
       <c r="C49" s="29"/>
@@ -5561,10 +5620,11 @@
       <c r="BB49" s="29"/>
       <c r="BC49" s="29"/>
       <c r="BD49" s="29"/>
-      <c r="BE49" s="30"/>
+      <c r="BE49" s="29"/>
       <c r="BF49" s="30"/>
-    </row>
-    <row r="50" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG49" s="30"/>
+    </row>
+    <row r="50" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="32"/>
       <c r="B50" s="33"/>
       <c r="C50" s="34"/>
@@ -5623,10 +5683,11 @@
       <c r="BD50" s="34"/>
       <c r="BE50" s="34"/>
       <c r="BF50" s="34"/>
+      <c r="BG50" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5653,10 +5714,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="84"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -5744,10 +5805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV98"/>
+  <dimension ref="A1:IV99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5761,16 +5822,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="89" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="87"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -5779,16 +5840,16 @@
       <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90" t="s">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="92" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -5810,7 +5871,7 @@
       <c r="E3" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="83" t="s">
         <v>125</v>
       </c>
       <c r="G3" s="48" t="s">
@@ -5848,7 +5909,7 @@
       <c r="G4" s="62">
         <v>60</v>
       </c>
-      <c r="H4" s="94">
+      <c r="H4" s="84">
         <v>0.35416666666666669</v>
       </c>
       <c r="I4" s="37"/>
@@ -5921,10 +5982,10 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="59"/>
       <c r="B8" s="54" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="D8" s="56"/>
       <c r="E8" s="56"/>
@@ -5941,10 +6002,10 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="59"/>
       <c r="B9" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="56"/>
       <c r="E9" s="56"/>
@@ -5961,10 +6022,10 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="B10" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="56"/>
       <c r="E10" s="56"/>
@@ -5981,10 +6042,10 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="B11" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="56"/>
@@ -6001,10 +6062,10 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="B12" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
@@ -6021,10 +6082,10 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="B13" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="56"/>
       <c r="E13" s="56"/>
@@ -6041,10 +6102,10 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="B14" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
@@ -6061,10 +6122,10 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="B15" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="56"/>
@@ -6081,10 +6142,10 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="59"/>
       <c r="B16" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
@@ -6101,10 +6162,10 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="59"/>
       <c r="B17" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
@@ -6121,10 +6182,10 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="59"/>
       <c r="B18" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
@@ -6141,10 +6202,10 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="59"/>
       <c r="B19" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
@@ -6161,10 +6222,10 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="59"/>
       <c r="B20" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
@@ -6181,10 +6242,10 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="59"/>
       <c r="B21" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
@@ -6201,10 +6262,10 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="59"/>
       <c r="B22" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
@@ -6221,10 +6282,10 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="59"/>
       <c r="B23" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
@@ -6241,10 +6302,10 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="59"/>
       <c r="B24" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
@@ -6261,10 +6322,10 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="59"/>
       <c r="B25" s="54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
@@ -6281,10 +6342,10 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="59"/>
       <c r="B26" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
@@ -6301,10 +6362,10 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="59"/>
       <c r="B27" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
@@ -6321,10 +6382,10 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="59"/>
       <c r="B28" s="54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
@@ -6341,10 +6402,10 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="59"/>
       <c r="B29" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
@@ -6361,10 +6422,10 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="59"/>
       <c r="B30" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="56"/>
       <c r="E30" s="56"/>
@@ -6381,10 +6442,10 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="59"/>
       <c r="B31" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="55" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="56"/>
       <c r="E31" s="56"/>
@@ -6401,10 +6462,10 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="59"/>
       <c r="B32" s="54" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
@@ -6421,10 +6482,10 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="59"/>
       <c r="B33" s="54" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="56"/>
       <c r="E33" s="56"/>
@@ -6441,10 +6502,10 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="59"/>
       <c r="B34" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
@@ -6461,10 +6522,10 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="59"/>
       <c r="B35" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="56"/>
       <c r="E35" s="56"/>
@@ -6481,10 +6542,10 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="59"/>
       <c r="B36" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
@@ -6501,10 +6562,10 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="59"/>
       <c r="B37" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="56"/>
       <c r="E37" s="56"/>
@@ -6521,10 +6582,10 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="59"/>
       <c r="B38" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="56"/>
       <c r="E38" s="56"/>
@@ -6541,10 +6602,10 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="59"/>
       <c r="B39" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
@@ -6561,10 +6622,10 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="59"/>
       <c r="B40" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
@@ -6581,10 +6642,10 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="59"/>
       <c r="B41" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="56"/>
       <c r="E41" s="56"/>
@@ -6601,10 +6662,10 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="59"/>
       <c r="B42" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
@@ -6621,10 +6682,10 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="59"/>
       <c r="B43" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
@@ -6641,10 +6702,10 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="59"/>
       <c r="B44" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
@@ -6661,10 +6722,10 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="59"/>
       <c r="B45" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="56"/>
       <c r="E45" s="56"/>
@@ -6681,10 +6742,10 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="59"/>
       <c r="B46" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
@@ -6701,10 +6762,10 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="59"/>
       <c r="B47" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" s="56"/>
       <c r="E47" s="56"/>
@@ -6721,10 +6782,10 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="59"/>
       <c r="B48" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" s="55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
@@ -6741,10 +6802,10 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="59"/>
       <c r="B49" s="54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" s="56"/>
       <c r="E49" s="56"/>
@@ -6761,10 +6822,10 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="59"/>
       <c r="B50" s="54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
@@ -6781,10 +6842,10 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="59"/>
       <c r="B51" s="54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" s="55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" s="56"/>
       <c r="E51" s="56"/>
@@ -6801,10 +6862,10 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="59"/>
       <c r="B52" s="54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" s="55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="56"/>
       <c r="E52" s="56"/>
@@ -6821,10 +6882,10 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="59"/>
       <c r="B53" s="54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53" s="56"/>
       <c r="E53" s="56"/>
@@ -6841,10 +6902,10 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="59"/>
       <c r="B54" s="54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" s="55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" s="56"/>
       <c r="E54" s="56"/>
@@ -6861,10 +6922,10 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="59"/>
       <c r="B55" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D55" s="56"/>
       <c r="E55" s="56"/>
@@ -6881,10 +6942,10 @@
     <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="59"/>
       <c r="B56" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" s="55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="56"/>
       <c r="E56" s="56"/>
@@ -6901,10 +6962,10 @@
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="59"/>
       <c r="B57" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" s="55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" s="56"/>
       <c r="E57" s="56"/>
@@ -6921,10 +6982,10 @@
     <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="59"/>
       <c r="B58" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="56"/>
       <c r="E58" s="56"/>
@@ -6941,10 +7002,10 @@
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="59"/>
       <c r="B59" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="56"/>
       <c r="E59" s="56"/>
@@ -6960,14 +7021,14 @@
     </row>
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="59"/>
-      <c r="B60" s="78" t="s">
-        <v>120</v>
-      </c>
-      <c r="C60" s="79" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" s="80"/>
-      <c r="E60" s="80"/>
+      <c r="B60" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
       <c r="H60" s="37"/>
@@ -6980,10 +7041,14 @@
     </row>
     <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="59"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="63"/>
+      <c r="B61" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" s="80"/>
+      <c r="E61" s="80"/>
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
       <c r="H61" s="37"/>
@@ -7078,7 +7143,7 @@
       <c r="A67" s="59"/>
       <c r="B67" s="36"/>
       <c r="C67" s="37"/>
-      <c r="D67" s="56"/>
+      <c r="D67" s="60"/>
       <c r="E67" s="63"/>
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
@@ -7571,7 +7636,7 @@
       <c r="N97" s="37"/>
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="61"/>
+      <c r="A98" s="59"/>
       <c r="B98" s="36"/>
       <c r="C98" s="37"/>
       <c r="D98" s="56"/>
@@ -7586,6 +7651,22 @@
       <c r="M98" s="37"/>
       <c r="N98" s="37"/>
     </row>
+    <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="61"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="63"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
+      <c r="K99" s="37"/>
+      <c r="L99" s="37"/>
+      <c r="M99" s="37"/>
+      <c r="N99" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>

</xml_diff>